<commit_message>
ZRV2.5 file upload and cleanup for release
</commit_message>
<xml_diff>
--- a/bom/BOM_ZR_V2.5.xlsx
+++ b/bom/BOM_ZR_V2.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243A3957-A8A0-4ECC-9D76-9C96A078DD89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F41775-6781-4AEA-B122-F2B2B1AA0AD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -884,20 +884,6 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -923,6 +909,20 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3759,13 +3759,13 @@
     <tableColumn id="2" xr3:uid="{8D81458F-CC8E-4FB2-AC08-34D35D773E2C}" name="Category" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{B9E559F2-25D5-4277-BB75-76856C22B650}" name="Item" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{88B61831-5965-4EF9-94F1-EFD61EC76829}" name="Thumbnail" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{57668B42-82FE-40E2-B7EE-58DA6BBEBF56}" name="Part Name" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{0BCBCD91-246F-43A0-B8C5-04E596E69EEA}" name="Part Description" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{ACE43926-E340-4876-958D-0EF54DCBE9FA}" name="Make/Buy" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{DA7121B7-FA12-4C8D-991C-7770D7553E03}" name="QTY" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{F3D31371-2653-4B6C-8EF2-EBF3EDB7638C}" name="Comment" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{97C0D926-0B05-4BCC-BC0C-84F1540EE5F0}" name="Vendor" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{E5A8160D-7E28-49C9-8F1D-EB7E0F628E21}" name="Vendor URL" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{57668B42-82FE-40E2-B7EE-58DA6BBEBF56}" name="Part Name" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{0BCBCD91-246F-43A0-B8C5-04E596E69EEA}" name="Part Description" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{ACE43926-E340-4876-958D-0EF54DCBE9FA}" name="Make/Buy" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{DA7121B7-FA12-4C8D-991C-7770D7553E03}" name="QTY" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{F3D31371-2653-4B6C-8EF2-EBF3EDB7638C}" name="Comment" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{97C0D926-0B05-4BCC-BC0C-84F1540EE5F0}" name="Vendor" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{E5A8160D-7E28-49C9-8F1D-EB7E0F628E21}" name="Vendor URL" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4095,8 +4095,8 @@
   <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="84.65" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5976,7 +5976,7 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
   <drawing r:id="rId4"/>
   <webPublishItems count="1">
-    <webPublishItem id="6083" divId="BOM_ZR_V2_6083" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_ZR_V2.htm" autoRepublish="1"/>
+    <webPublishItem id="6083" divId="BOM_ZR_V2_6083" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_ZR_V2.5.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
     <tablePart r:id="rId5"/>

</xml_diff>

<commit_message>
ZR2.5_Bom and STL added
</commit_message>
<xml_diff>
--- a/bom/BOM_ZR_V2.5.xlsx
+++ b/bom/BOM_ZR_V2.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F41775-6781-4AEA-B122-F2B2B1AA0AD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AB58AA-248C-477B-ADF7-8DA8F95979B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="198">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -534,9 +534,6 @@
   </si>
   <si>
     <t>Thingiverse</t>
-  </si>
-  <si>
-    <t>https://www.thingiverse.com/thing:4387638</t>
   </si>
   <si>
     <t>To be used with 48mm Stepper and Double Thrust Bearing Motor Mounts.</t>
@@ -591,9 +588,6 @@
     <t>BK10 and BF10 machined end required.   BK10 and BF10 blocks ARE NOT required.</t>
   </si>
   <si>
-    <t>Ball Bearing dont need to be magnetized, Stainless Steal or Chrome Steal preffered.</t>
-  </si>
-  <si>
     <t>ZR_MotorMount_RR_Body_V2.5</t>
   </si>
   <si>
@@ -643,6 +637,12 @@
   </si>
   <si>
     <t>Washer, M10X18X1.5</t>
+  </si>
+  <si>
+    <t>Ball Bearing dont need to be magnetized, Chrome Steal preffered.</t>
+  </si>
+  <si>
+    <t>HevORT/files/STL/ZR_V2.5 at master · MirageC79/HevORT (github.com)</t>
   </si>
 </sst>
 </file>
@@ -744,7 +744,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -754,12 +754,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,9 +844,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -874,7 +865,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4095,21 +4089,21 @@
   <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="84.65" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.453125" style="14"/>
-    <col min="2" max="2" width="16.453125" style="15"/>
+    <col min="1" max="1" width="16.453125" style="13"/>
+    <col min="2" max="2" width="16.453125" style="14"/>
     <col min="3" max="3" width="16.453125" style="9"/>
     <col min="4" max="4" width="20.7265625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="44.81640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49" style="19" customWidth="1"/>
+    <col min="5" max="5" width="44.81640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49" style="18" customWidth="1"/>
     <col min="7" max="7" width="14.81640625" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.453125" style="8"/>
-    <col min="9" max="9" width="56.1796875" style="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="56.1796875" style="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.453125" style="6"/>
     <col min="11" max="11" width="39.81640625" style="6" customWidth="1"/>
     <col min="12" max="12" width="33.81640625" style="6" hidden="1" customWidth="1"/>
@@ -4155,19 +4149,19 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B2" s="15" t="s">
+      <c r="A2" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>89</v>
       </c>
       <c r="G2" s="9" t="s">
@@ -4176,7 +4170,7 @@
       <c r="H2" s="8">
         <v>1</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>162</v>
       </c>
       <c r="L2" s="6" t="s">
@@ -4184,19 +4178,19 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="9">
         <v>2</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="18" t="s">
         <v>95</v>
       </c>
       <c r="G3" s="9" t="s">
@@ -4205,27 +4199,27 @@
       <c r="H3" s="8">
         <v>4</v>
       </c>
-      <c r="I3" s="21" t="s">
-        <v>178</v>
+      <c r="I3" s="20" t="s">
+        <v>177</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="9">
         <v>3</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="19" t="s">
+      <c r="F4" s="18" t="s">
         <v>17</v>
       </c>
       <c r="G4" s="9" t="s">
@@ -4234,27 +4228,27 @@
       <c r="H4" s="8">
         <v>3</v>
       </c>
-      <c r="I4" s="21" t="s">
-        <v>179</v>
+      <c r="I4" s="20" t="s">
+        <v>178</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B5" s="15" t="s">
+      <c r="A5" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="9">
         <v>4</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="18" t="s">
         <v>161</v>
       </c>
       <c r="G5" s="9" t="s">
@@ -4268,21 +4262,21 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="9">
         <v>5</v>
       </c>
       <c r="D6" s="10"/>
-      <c r="E6" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>186</v>
+      <c r="E6" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>184</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>6</v>
@@ -4290,7 +4284,7 @@
       <c r="H6" s="12">
         <v>3</v>
       </c>
-      <c r="I6" s="18"/>
+      <c r="I6" s="17"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="6" t="s">
@@ -4298,21 +4292,21 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B7" s="16" t="s">
+      <c r="A7" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="9">
         <v>6</v>
       </c>
       <c r="D7" s="10"/>
-      <c r="E7" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>188</v>
+      <c r="E7" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>186</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>6</v>
@@ -4320,24 +4314,24 @@
       <c r="H7" s="12">
         <v>3</v>
       </c>
-      <c r="I7" s="18"/>
+      <c r="I7" s="17"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
     </row>
     <row r="8" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="9">
         <v>7</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="19" t="s">
+      <c r="F8" s="18" t="s">
         <v>20</v>
       </c>
       <c r="G8" s="9" t="s">
@@ -4351,19 +4345,19 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B9" s="15" t="s">
+      <c r="A9" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="9">
         <v>8</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="18" t="s">
         <v>112</v>
       </c>
       <c r="G9" s="9" t="s">
@@ -4377,19 +4371,19 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B10" s="15" t="s">
+      <c r="A10" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="9">
         <v>9</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="18" t="s">
         <v>137</v>
       </c>
       <c r="G10" s="9" t="s">
@@ -4398,7 +4392,7 @@
       <c r="H10" s="8">
         <v>3</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="16" t="s">
         <v>162</v>
       </c>
       <c r="L10" s="6" t="s">
@@ -4406,19 +4400,19 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B11" s="15" t="s">
+      <c r="A11" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="9">
         <v>10</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="18" t="s">
         <v>86</v>
       </c>
       <c r="G11" s="9" t="s">
@@ -4427,30 +4421,30 @@
       <c r="H11" s="8">
         <v>1</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="K11" s="17" t="s">
-        <v>177</v>
+      <c r="K11" s="16" t="s">
+        <v>176</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B12" s="15" t="s">
+      <c r="A12" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="9">
         <v>11</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="18" t="s">
         <v>114</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="18" t="s">
         <v>115</v>
       </c>
       <c r="G12" s="9" t="s">
@@ -4464,19 +4458,19 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B13" s="15" t="s">
+      <c r="A13" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="9">
         <v>12</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="18" t="s">
         <v>9</v>
       </c>
       <c r="G13" s="9" t="s">
@@ -4485,7 +4479,7 @@
       <c r="H13" s="8">
         <v>3</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="16" t="s">
         <v>163</v>
       </c>
       <c r="L13" s="6" t="s">
@@ -4493,19 +4487,19 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B14" s="15" t="s">
+      <c r="A14" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C14" s="9">
         <v>13</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="F14" s="18" t="s">
         <v>81</v>
       </c>
       <c r="G14" s="9" t="s">
@@ -4514,28 +4508,28 @@
       <c r="H14" s="8">
         <v>9</v>
       </c>
-      <c r="I14" s="21" t="s">
-        <v>180</v>
+      <c r="I14" s="20" t="s">
+        <v>196</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C15" s="9">
         <v>14</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="F15" s="18" t="s">
         <v>171</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>172</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>6</v>
@@ -4543,27 +4537,27 @@
       <c r="H15" s="8">
         <v>30</v>
       </c>
-      <c r="I15" s="17" t="s">
-        <v>173</v>
+      <c r="I15" s="16" t="s">
+        <v>172</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B16" s="15" t="s">
+      <c r="A16" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C16" s="9">
         <v>15</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="18" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="9" t="s">
@@ -4572,7 +4566,7 @@
       <c r="H16" s="8">
         <v>3</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="I16" s="16" t="s">
         <v>164</v>
       </c>
       <c r="L16" s="6" t="s">
@@ -4580,20 +4574,20 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B17" s="15" t="s">
+      <c r="A17" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C17" s="9">
         <v>16</v>
       </c>
-      <c r="E17" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>197</v>
+      <c r="E17" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>195</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>6</v>
@@ -4603,19 +4597,19 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B18" s="15" t="s">
+      <c r="A18" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C18" s="9">
         <v>17</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="F18" s="18" t="s">
         <v>70</v>
       </c>
       <c r="G18" s="9" t="s">
@@ -4629,19 +4623,19 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C19" s="9">
         <v>18</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="18" t="s">
         <v>75</v>
       </c>
       <c r="G19" s="9" t="s">
@@ -4655,19 +4649,19 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B20" s="15" t="s">
+      <c r="A20" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C20" s="9">
         <v>19</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F20" s="18" t="s">
         <v>52</v>
       </c>
       <c r="G20" s="9" t="s">
@@ -4681,19 +4675,19 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B21" s="15" t="s">
+      <c r="A21" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C21" s="9">
         <v>20</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="F21" s="19" t="s">
+      <c r="F21" s="18" t="s">
         <v>118</v>
       </c>
       <c r="G21" s="9" t="s">
@@ -4702,7 +4696,7 @@
       <c r="H21" s="8">
         <v>26</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="16" t="s">
         <v>165</v>
       </c>
       <c r="L21" s="6" t="s">
@@ -4710,20 +4704,20 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B22" s="15" t="s">
+      <c r="A22" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C22" s="9">
         <v>21</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="F22" s="19" t="s">
-        <v>175</v>
+      <c r="F22" s="18" t="s">
+        <v>174</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>6</v>
@@ -4731,27 +4725,27 @@
       <c r="H22" s="8">
         <v>24</v>
       </c>
-      <c r="I22" s="17" t="s">
-        <v>176</v>
+      <c r="I22" s="16" t="s">
+        <v>175</v>
       </c>
       <c r="L22" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B23" s="15" t="s">
+      <c r="A23" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C23" s="9">
         <v>22</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="18" t="s">
         <v>134</v>
       </c>
       <c r="G23" s="9" t="s">
@@ -4760,7 +4754,7 @@
       <c r="H23" s="8">
         <v>6</v>
       </c>
-      <c r="I23" s="17" t="s">
+      <c r="I23" s="16" t="s">
         <v>165</v>
       </c>
       <c r="L23" s="6" t="s">
@@ -4768,19 +4762,19 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B24" s="15" t="s">
+      <c r="A24" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B24" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C24" s="9">
         <v>23</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="F24" s="18" t="s">
         <v>29</v>
       </c>
       <c r="G24" s="9" t="s">
@@ -4789,7 +4783,7 @@
       <c r="H24" s="8">
         <v>15</v>
       </c>
-      <c r="I24" s="17" t="s">
+      <c r="I24" s="16" t="s">
         <v>165</v>
       </c>
       <c r="L24" s="6" t="s">
@@ -4797,19 +4791,19 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B25" s="15" t="s">
+      <c r="A25" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B25" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C25" s="9">
         <v>24</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="19" t="s">
+      <c r="F25" s="18" t="s">
         <v>35</v>
       </c>
       <c r="G25" s="9" t="s">
@@ -4823,19 +4817,19 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B26" s="15" t="s">
+      <c r="A26" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C26" s="9">
         <v>25</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="F26" s="19" t="s">
+      <c r="F26" s="18" t="s">
         <v>101</v>
       </c>
       <c r="G26" s="9" t="s">
@@ -4849,19 +4843,19 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B27" s="15" t="s">
+      <c r="A27" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B27" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C27" s="9">
         <v>26</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="F27" s="19" t="s">
+      <c r="F27" s="18" t="s">
         <v>141</v>
       </c>
       <c r="G27" s="9" t="s">
@@ -4875,19 +4869,19 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B28" s="15" t="s">
+      <c r="A28" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B28" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C28" s="9">
         <v>27</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="19" t="s">
+      <c r="F28" s="18" t="s">
         <v>32</v>
       </c>
       <c r="G28" s="9" t="s">
@@ -4901,19 +4895,19 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B29" s="15" t="s">
+      <c r="A29" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B29" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C29" s="9">
         <v>28</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="19" t="s">
+      <c r="F29" s="18" t="s">
         <v>46</v>
       </c>
       <c r="G29" s="9" t="s">
@@ -4927,19 +4921,19 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B30" s="15" t="s">
+      <c r="A30" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B30" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C30" s="9">
         <v>29</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="19" t="s">
+      <c r="F30" s="18" t="s">
         <v>26</v>
       </c>
       <c r="G30" s="9" t="s">
@@ -4953,19 +4947,19 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B31" s="15" t="s">
+      <c r="A31" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B31" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C31" s="9">
         <v>30</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="19" t="s">
+      <c r="F31" s="18" t="s">
         <v>40</v>
       </c>
       <c r="G31" s="9" t="s">
@@ -4979,20 +4973,20 @@
       </c>
     </row>
     <row r="32" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B32" s="15" t="s">
+      <c r="A32" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B32" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C32" s="9">
         <v>31</v>
       </c>
-      <c r="E32" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>195</v>
+      <c r="E32" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>193</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>6</v>
@@ -5002,19 +4996,19 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B33" s="15" t="s">
+      <c r="A33" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C33" s="9">
         <v>32</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="F33" s="19" t="s">
+      <c r="F33" s="18" t="s">
         <v>109</v>
       </c>
       <c r="G33" s="9" t="s">
@@ -5028,19 +5022,19 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B34" s="15" t="s">
+      <c r="A34" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B34" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C34" s="9">
         <v>33</v>
       </c>
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="F34" s="19" t="s">
+      <c r="F34" s="18" t="s">
         <v>78</v>
       </c>
       <c r="G34" s="9" t="s">
@@ -5054,19 +5048,19 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B35" s="15" t="s">
+      <c r="A35" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B35" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C35" s="9">
         <v>34</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F35" s="19" t="s">
+      <c r="F35" s="18" t="s">
         <v>49</v>
       </c>
       <c r="G35" s="9" t="s">
@@ -5080,19 +5074,19 @@
       </c>
     </row>
     <row r="36" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B36" s="15" t="s">
+      <c r="A36" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C36" s="9">
         <v>35</v>
       </c>
-      <c r="E36" s="19" t="s">
+      <c r="E36" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="18" t="s">
         <v>60</v>
       </c>
       <c r="G36" s="9" t="s">
@@ -5106,19 +5100,19 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B37" s="15" t="s">
+      <c r="A37" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B37" s="14" t="s">
         <v>159</v>
       </c>
       <c r="C37" s="9">
         <v>36</v>
       </c>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F37" s="19" t="s">
+      <c r="F37" s="18" t="s">
         <v>98</v>
       </c>
       <c r="G37" s="9" t="s">
@@ -5132,19 +5126,19 @@
       </c>
     </row>
     <row r="38" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B38" s="15" t="s">
+      <c r="A38" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B38" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="9">
         <v>37</v>
       </c>
-      <c r="E38" s="19" t="s">
+      <c r="E38" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="F38" s="19" t="s">
+      <c r="F38" s="18" t="s">
         <v>131</v>
       </c>
       <c r="G38" s="9" t="s">
@@ -5153,33 +5147,33 @@
       <c r="H38" s="8">
         <v>1</v>
       </c>
-      <c r="I38" s="17" t="s">
-        <v>170</v>
+      <c r="I38" s="16" t="s">
+        <v>169</v>
       </c>
       <c r="J38" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K38" s="13" t="s">
-        <v>168</v>
+      <c r="K38" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L38" s="6" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B39" s="15" t="s">
+      <c r="A39" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B39" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C39" s="9">
         <v>38</v>
       </c>
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="F39" s="19" t="s">
+      <c r="F39" s="18" t="s">
         <v>128</v>
       </c>
       <c r="G39" s="9" t="s">
@@ -5188,33 +5182,33 @@
       <c r="H39" s="8">
         <v>1</v>
       </c>
-      <c r="I39" s="17" t="s">
-        <v>170</v>
+      <c r="I39" s="16" t="s">
+        <v>169</v>
       </c>
       <c r="J39" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K39" s="13" t="s">
-        <v>168</v>
+      <c r="K39" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L39" s="6" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B40" s="15" t="s">
+      <c r="A40" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B40" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="9">
         <v>39</v>
       </c>
-      <c r="E40" s="19" t="s">
+      <c r="E40" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="F40" s="19" t="s">
+      <c r="F40" s="18" t="s">
         <v>55</v>
       </c>
       <c r="G40" s="9" t="s">
@@ -5223,34 +5217,34 @@
       <c r="H40" s="8">
         <v>3</v>
       </c>
-      <c r="I40" s="17" t="s">
-        <v>174</v>
+      <c r="I40" s="16" t="s">
+        <v>173</v>
       </c>
       <c r="J40" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K40" s="13" t="s">
-        <v>168</v>
+      <c r="K40" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L40" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B41" s="15" t="s">
+      <c r="A41" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B41" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C41" s="9">
         <v>40</v>
       </c>
-      <c r="E41" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="F41" s="19" t="s">
+      <c r="E41" s="18" t="s">
         <v>182</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>180</v>
       </c>
       <c r="G41" s="9" t="s">
         <v>11</v>
@@ -5261,28 +5255,28 @@
       <c r="J41" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K41" s="13" t="s">
-        <v>168</v>
+      <c r="K41" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L41" s="6" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B42" s="15" t="s">
+      <c r="A42" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B42" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="9">
         <v>41</v>
       </c>
-      <c r="E42" s="19" t="s">
+      <c r="E42" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="F42" s="18" t="s">
         <v>191</v>
-      </c>
-      <c r="F42" s="19" t="s">
-        <v>193</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>11</v>
@@ -5290,23 +5284,25 @@
       <c r="H42" s="8">
         <v>1</v>
       </c>
-      <c r="K42" s="13"/>
+      <c r="K42" s="21" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="43" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B43" s="15" t="s">
+      <c r="A43" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B43" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="9">
         <v>42</v>
       </c>
-      <c r="E43" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="F43" s="19" t="s">
-        <v>182</v>
+      <c r="E43" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="F43" s="18" t="s">
+        <v>180</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>11</v>
@@ -5317,28 +5313,28 @@
       <c r="J43" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K43" s="13" t="s">
-        <v>168</v>
+      <c r="K43" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L43" s="6" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B44" s="15" t="s">
+      <c r="A44" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B44" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C44" s="9">
         <v>43</v>
       </c>
-      <c r="E44" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="F44" s="19" t="s">
-        <v>193</v>
+      <c r="E44" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="F44" s="18" t="s">
+        <v>191</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>11</v>
@@ -5346,23 +5342,25 @@
       <c r="H44" s="8">
         <v>1</v>
       </c>
-      <c r="K44" s="13"/>
+      <c r="K44" s="21" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="45" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B45" s="15" t="s">
+      <c r="A45" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B45" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C45" s="9">
         <v>44</v>
       </c>
-      <c r="E45" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>182</v>
+      <c r="E45" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>180</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>11</v>
@@ -5373,28 +5371,28 @@
       <c r="J45" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K45" s="13" t="s">
-        <v>168</v>
+      <c r="K45" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L45" s="6" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B46" s="15" t="s">
+      <c r="A46" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B46" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C46" s="9">
         <v>45</v>
       </c>
-      <c r="E46" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="F46" s="19" t="s">
-        <v>193</v>
+      <c r="E46" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="F46" s="18" t="s">
+        <v>191</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>11</v>
@@ -5402,22 +5400,24 @@
       <c r="H46" s="8">
         <v>1</v>
       </c>
-      <c r="K46" s="13"/>
+      <c r="K46" s="21" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="47" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B47" s="15" t="s">
+      <c r="A47" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B47" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C47" s="9">
         <v>46</v>
       </c>
-      <c r="E47" s="19" t="s">
+      <c r="E47" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F47" s="19" t="s">
+      <c r="F47" s="18" t="s">
         <v>43</v>
       </c>
       <c r="G47" s="9" t="s">
@@ -5429,27 +5429,27 @@
       <c r="J47" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K47" s="13" t="s">
-        <v>168</v>
+      <c r="K47" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L47" s="6" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B48" s="15" t="s">
+      <c r="A48" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B48" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C48" s="9">
         <v>47</v>
       </c>
-      <c r="E48" s="19" t="s">
+      <c r="E48" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="F48" s="19" t="s">
+      <c r="F48" s="18" t="s">
         <v>43</v>
       </c>
       <c r="G48" s="9" t="s">
@@ -5461,27 +5461,27 @@
       <c r="J48" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K48" s="13" t="s">
-        <v>168</v>
+      <c r="K48" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L48" s="6" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B49" s="15" t="s">
+      <c r="A49" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B49" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C49" s="9">
         <v>48</v>
       </c>
-      <c r="E49" s="19" t="s">
+      <c r="E49" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="F49" s="19" t="s">
+      <c r="F49" s="18" t="s">
         <v>43</v>
       </c>
       <c r="G49" s="9" t="s">
@@ -5493,27 +5493,27 @@
       <c r="J49" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K49" s="13" t="s">
-        <v>168</v>
+      <c r="K49" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L49" s="6" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B50" s="15" t="s">
+      <c r="A50" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B50" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C50" s="9">
         <v>49</v>
       </c>
-      <c r="E50" s="19" t="s">
+      <c r="E50" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="F50" s="19" t="s">
+      <c r="F50" s="18" t="s">
         <v>106</v>
       </c>
       <c r="G50" s="9" t="s">
@@ -5525,27 +5525,27 @@
       <c r="J50" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K50" s="13" t="s">
-        <v>168</v>
+      <c r="K50" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L50" s="6" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B51" s="15" t="s">
+      <c r="A51" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B51" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C51" s="9">
         <v>50</v>
       </c>
-      <c r="E51" s="19" t="s">
+      <c r="E51" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F51" s="19" t="s">
+      <c r="F51" s="18" t="s">
         <v>84</v>
       </c>
       <c r="G51" s="9" t="s">
@@ -5557,27 +5557,27 @@
       <c r="J51" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K51" s="13" t="s">
-        <v>168</v>
+      <c r="K51" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L51" s="6" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B52" s="15" t="s">
+      <c r="A52" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B52" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C52" s="9">
         <v>51</v>
       </c>
-      <c r="E52" s="19" t="s">
+      <c r="E52" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F52" s="19" t="s">
+      <c r="F52" s="18" t="s">
         <v>67</v>
       </c>
       <c r="G52" s="9" t="s">
@@ -5589,27 +5589,27 @@
       <c r="J52" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K52" s="13" t="s">
-        <v>168</v>
+      <c r="K52" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L52" s="6" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B53" s="15" t="s">
+      <c r="A53" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B53" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C53" s="9">
         <v>52</v>
       </c>
-      <c r="E53" s="19" t="s">
+      <c r="E53" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="F53" s="19" t="s">
+      <c r="F53" s="18" t="s">
         <v>166</v>
       </c>
       <c r="G53" s="9" t="s">
@@ -5621,27 +5621,27 @@
       <c r="J53" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K53" s="13" t="s">
-        <v>168</v>
+      <c r="K53" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L53" s="6" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B54" s="15" t="s">
+      <c r="A54" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B54" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C54" s="9">
         <v>53</v>
       </c>
-      <c r="E54" s="19" t="s">
+      <c r="E54" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F54" s="19" t="s">
+      <c r="F54" s="18" t="s">
         <v>23</v>
       </c>
       <c r="G54" s="9" t="s">
@@ -5650,33 +5650,33 @@
       <c r="H54" s="8">
         <v>4</v>
       </c>
-      <c r="I54" s="17" t="s">
-        <v>174</v>
+      <c r="I54" s="16" t="s">
+        <v>173</v>
       </c>
       <c r="J54" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K54" s="13" t="s">
-        <v>168</v>
+      <c r="K54" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L54" s="6" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B55" s="15" t="s">
+      <c r="A55" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C55" s="9">
         <v>54</v>
       </c>
-      <c r="E55" s="19" t="s">
+      <c r="E55" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="F55" s="19" t="s">
+      <c r="F55" s="18" t="s">
         <v>64</v>
       </c>
       <c r="G55" s="9" t="s">
@@ -5685,33 +5685,33 @@
       <c r="H55" s="8">
         <v>2</v>
       </c>
-      <c r="I55" s="17" t="s">
-        <v>174</v>
+      <c r="I55" s="16" t="s">
+        <v>173</v>
       </c>
       <c r="J55" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K55" s="13" t="s">
-        <v>168</v>
+      <c r="K55" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L55" s="6" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B56" s="15" t="s">
+      <c r="A56" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B56" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C56" s="9">
         <v>55</v>
       </c>
-      <c r="E56" s="19" t="s">
+      <c r="E56" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="F56" s="19" t="s">
+      <c r="F56" s="18" t="s">
         <v>144</v>
       </c>
       <c r="G56" s="9" t="s">
@@ -5720,33 +5720,33 @@
       <c r="H56" s="8">
         <v>1</v>
       </c>
-      <c r="I56" s="17" t="s">
-        <v>169</v>
+      <c r="I56" s="16" t="s">
+        <v>168</v>
       </c>
       <c r="J56" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K56" s="13" t="s">
-        <v>168</v>
+      <c r="K56" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L56" s="6" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B57" s="15" t="s">
+      <c r="A57" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B57" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C57" s="9">
         <v>56</v>
       </c>
-      <c r="E57" s="19" t="s">
+      <c r="E57" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="F57" s="19" t="s">
+      <c r="F57" s="18" t="s">
         <v>148</v>
       </c>
       <c r="G57" s="9" t="s">
@@ -5755,33 +5755,33 @@
       <c r="H57" s="8">
         <v>1</v>
       </c>
-      <c r="I57" s="17" t="s">
-        <v>169</v>
+      <c r="I57" s="16" t="s">
+        <v>168</v>
       </c>
       <c r="J57" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K57" s="13" t="s">
-        <v>168</v>
+      <c r="K57" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L57" s="6" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B58" s="15" t="s">
+      <c r="A58" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B58" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C58" s="9">
         <v>57</v>
       </c>
-      <c r="E58" s="19" t="s">
+      <c r="E58" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="F58" s="19" t="s">
+      <c r="F58" s="18" t="s">
         <v>151</v>
       </c>
       <c r="G58" s="9" t="s">
@@ -5790,33 +5790,33 @@
       <c r="H58" s="8">
         <v>1</v>
       </c>
-      <c r="I58" s="17" t="s">
-        <v>169</v>
+      <c r="I58" s="16" t="s">
+        <v>168</v>
       </c>
       <c r="J58" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K58" s="13" t="s">
-        <v>168</v>
+      <c r="K58" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L58" s="6" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B59" s="15" t="s">
+      <c r="A59" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B59" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C59" s="9">
         <v>58</v>
       </c>
-      <c r="E59" s="19" t="s">
+      <c r="E59" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="F59" s="19" t="s">
+      <c r="F59" s="18" t="s">
         <v>120</v>
       </c>
       <c r="G59" s="9" t="s">
@@ -5825,33 +5825,33 @@
       <c r="H59" s="8">
         <v>1</v>
       </c>
-      <c r="I59" s="17" t="s">
-        <v>170</v>
+      <c r="I59" s="16" t="s">
+        <v>169</v>
       </c>
       <c r="J59" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K59" s="13" t="s">
-        <v>168</v>
+      <c r="K59" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L59" s="6" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B60" s="15" t="s">
+      <c r="A60" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B60" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C60" s="9">
         <v>59</v>
       </c>
-      <c r="E60" s="19" t="s">
+      <c r="E60" s="18" t="s">
         <v>103</v>
       </c>
-      <c r="F60" s="19" t="s">
+      <c r="F60" s="18" t="s">
         <v>103</v>
       </c>
       <c r="G60" s="9" t="s">
@@ -5863,27 +5863,27 @@
       <c r="J60" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K60" s="13" t="s">
-        <v>168</v>
+      <c r="K60" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L60" s="6" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B61" s="15" t="s">
+      <c r="A61" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B61" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C61" s="9">
         <v>60</v>
       </c>
-      <c r="E61" s="19" t="s">
+      <c r="E61" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="F61" s="19" t="s">
+      <c r="F61" s="18" t="s">
         <v>160</v>
       </c>
       <c r="G61" s="9" t="s">
@@ -5895,24 +5895,24 @@
       <c r="J61" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K61" s="13" t="s">
-        <v>168</v>
+      <c r="K61" s="21" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B62" s="15" t="s">
+      <c r="A62" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B62" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C62" s="9">
         <v>61</v>
       </c>
-      <c r="E62" s="19" t="s">
+      <c r="E62" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="F62" s="19" t="s">
+      <c r="F62" s="18" t="s">
         <v>92</v>
       </c>
       <c r="G62" s="9" t="s">
@@ -5921,33 +5921,33 @@
       <c r="H62" s="8">
         <v>1</v>
       </c>
-      <c r="I62" s="17" t="s">
-        <v>170</v>
+      <c r="I62" s="16" t="s">
+        <v>169</v>
       </c>
       <c r="J62" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K62" s="13" t="s">
-        <v>168</v>
+      <c r="K62" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L62" s="6" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="B63" s="15" t="s">
+      <c r="A63" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B63" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C63" s="9">
         <v>62</v>
       </c>
-      <c r="E63" s="19" t="s">
+      <c r="E63" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="F63" s="19" t="s">
+      <c r="F63" s="18" t="s">
         <v>125</v>
       </c>
       <c r="G63" s="9" t="s">
@@ -5959,8 +5959,8 @@
       <c r="J63" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="K63" s="13" t="s">
-        <v>168</v>
+      <c r="K63" s="21" t="s">
+        <v>197</v>
       </c>
       <c r="L63" s="6" t="s">
         <v>152</v>
@@ -5969,17 +5969,19 @@
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="K38" r:id="rId1" xr:uid="{2D35E292-AF84-4ACA-8AB3-1DD7C1BB327A}"/>
-    <hyperlink ref="K39:K63" r:id="rId2" display="https://www.thingiverse.com/thing:4387638" xr:uid="{EEF9807B-3530-49F1-8A95-10297D8661DC}"/>
+    <hyperlink ref="K40" r:id="rId1" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/ZR_V2.5" xr:uid="{3B66D28E-F96D-4F18-B574-151B58D0E5C9}"/>
+    <hyperlink ref="K41:K63" r:id="rId2" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/ZR_V2.5" xr:uid="{0584AA04-59D9-4ACB-9F4E-9BC30A0C080A}"/>
+    <hyperlink ref="K38" r:id="rId3" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/ZR_V2.5" xr:uid="{E14FDDA0-4320-44DC-A169-67D9CC483D3D}"/>
+    <hyperlink ref="K39" r:id="rId4" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/ZR_V2.5" xr:uid="{E8CDD8F3-900B-4577-BD6C-D79B27C34BF0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
+  <drawing r:id="rId6"/>
   <webPublishItems count="1">
     <webPublishItem id="6083" divId="BOM_ZR_V2_6083" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_ZR_V2.5.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Recommended Stepper motor for Z
1.8 degree 60mm recommended.  The more Detent torque the better .
</commit_message>
<xml_diff>
--- a/bom/BOM_ZR_V2.5.xlsx
+++ b/bom/BOM_ZR_V2.5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEACA8F-7E3D-4AF2-A587-A2DCD9D4D41E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4388AB4-FDB9-44CD-974C-0E85A91BA427}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="16530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="From Fusion 360" sheetId="1" r:id="rId1"/>
@@ -56,12 +56,6 @@
     <t>2ef9a3e4130b47ff87e0a150cef27583</t>
   </si>
   <si>
-    <t>NEMA17_E3D_High_Torque_48mm</t>
-  </si>
-  <si>
-    <t>Stepper Motor - NEMA17X48mm</t>
-  </si>
-  <si>
     <t>e404c2ce27d244b19210a1bb56156199</t>
   </si>
   <si>
@@ -519,9 +513,6 @@
   </si>
   <si>
     <t>See required Dimension as per Frame Calculator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Can also use 40mm motor with 1.8 deg </t>
   </si>
   <si>
     <t>Thread has to be 1.00 to match Ball Screw machined end for BK10</t>
@@ -649,6 +640,15 @@
   </si>
   <si>
     <t>Amazon</t>
+  </si>
+  <si>
+    <t>NEMA17 1.8 degree Stepper Motors 60 mm*</t>
+  </si>
+  <si>
+    <t>*It is recommended to use 60mm 1.8 degree motors to avoid the bed falling down due to backdriving</t>
+  </si>
+  <si>
+    <t>Stepper Motor - NEMA17X60mm</t>
   </si>
 </sst>
 </file>
@@ -4098,8 +4098,8 @@
   <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E13" sqref="E13:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="84.65" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4121,13 +4121,13 @@
   <sheetData>
     <row r="1" spans="1:12" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -4136,16 +4136,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>3</v>
@@ -4159,7 +4159,7 @@
     </row>
     <row r="2" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>6</v>
@@ -4168,10 +4168,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>6</v>
@@ -4180,7 +4180,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>7</v>
@@ -4188,7 +4188,7 @@
     </row>
     <row r="3" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>6</v>
@@ -4197,10 +4197,10 @@
         <v>2</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>6</v>
@@ -4209,15 +4209,15 @@
         <v>4</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="L3" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>6</v>
@@ -4226,10 +4226,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>6</v>
@@ -4238,15 +4238,15 @@
         <v>3</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>6</v>
@@ -4255,10 +4255,10 @@
         <v>4</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>6</v>
@@ -4267,12 +4267,12 @@
         <v>3</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>6</v>
@@ -4282,10 +4282,10 @@
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="19" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>6</v>
@@ -4297,12 +4297,12 @@
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
       <c r="L6" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>6</v>
@@ -4312,10 +4312,10 @@
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="19" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>6</v>
@@ -4329,7 +4329,7 @@
     </row>
     <row r="8" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>6</v>
@@ -4338,10 +4338,10 @@
         <v>7</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>6</v>
@@ -4350,12 +4350,12 @@
         <v>3</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>6</v>
@@ -4364,10 +4364,10 @@
         <v>8</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>6</v>
@@ -4376,12 +4376,12 @@
         <v>3</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>6</v>
@@ -4390,10 +4390,10 @@
         <v>9</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F10" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>6</v>
@@ -4402,15 +4402,15 @@
         <v>3</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>6</v>
@@ -4419,10 +4419,10 @@
         <v>10</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>6</v>
@@ -4431,18 +4431,18 @@
         <v>1</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>6</v>
@@ -4451,10 +4451,10 @@
         <v>11</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F12" s="18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>6</v>
@@ -4463,12 +4463,12 @@
         <v>3</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>6</v>
@@ -4477,10 +4477,10 @@
         <v>12</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>8</v>
+        <v>197</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>9</v>
+        <v>199</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>6</v>
@@ -4489,27 +4489,27 @@
         <v>3</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>163</v>
+        <v>198</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C14" s="9">
         <v>13</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>6</v>
@@ -4518,27 +4518,27 @@
         <v>9</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C15" s="9">
         <v>14</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F15" s="18" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>6</v>
@@ -4547,33 +4547,33 @@
         <v>30</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="K15" s="22" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C16" s="9">
         <v>15</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F16" s="18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>6</v>
@@ -4582,27 +4582,27 @@
         <v>3</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C17" s="9">
         <v>16</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>6</v>
@@ -4613,19 +4613,19 @@
     </row>
     <row r="18" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C18" s="9">
         <v>17</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F18" s="18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>6</v>
@@ -4634,24 +4634,24 @@
         <v>22</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C19" s="9">
         <v>18</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F19" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>6</v>
@@ -4660,24 +4660,24 @@
         <v>9</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C20" s="9">
         <v>19</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>6</v>
@@ -4686,24 +4686,24 @@
         <v>6</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C21" s="9">
         <v>20</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>6</v>
@@ -4712,27 +4712,27 @@
         <v>26</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C22" s="9">
         <v>21</v>
       </c>
       <c r="E22" s="18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F22" s="18" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>6</v>
@@ -4741,27 +4741,27 @@
         <v>24</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C23" s="9">
         <v>22</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>6</v>
@@ -4770,27 +4770,27 @@
         <v>6</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C24" s="9">
         <v>23</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F24" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>6</v>
@@ -4799,27 +4799,27 @@
         <v>15</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C25" s="9">
         <v>24</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>6</v>
@@ -4828,24 +4828,24 @@
         <v>3</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C26" s="9">
         <v>25</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F26" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>6</v>
@@ -4854,24 +4854,24 @@
         <v>26</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C27" s="9">
         <v>26</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F27" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>6</v>
@@ -4880,24 +4880,24 @@
         <v>6</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C28" s="9">
         <v>27</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F28" s="18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>6</v>
@@ -4906,24 +4906,24 @@
         <v>16</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C29" s="9">
         <v>28</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F29" s="18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G29" s="9" t="s">
         <v>6</v>
@@ -4932,24 +4932,24 @@
         <v>46</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C30" s="9">
         <v>29</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F30" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>6</v>
@@ -4958,24 +4958,24 @@
         <v>18</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C31" s="9">
         <v>30</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F31" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G31" s="9" t="s">
         <v>6</v>
@@ -4984,24 +4984,24 @@
         <v>4</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C32" s="9">
         <v>31</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F32" s="18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>6</v>
@@ -5012,19 +5012,19 @@
     </row>
     <row r="33" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C33" s="9">
         <v>32</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F33" s="18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G33" s="9" t="s">
         <v>6</v>
@@ -5033,24 +5033,24 @@
         <v>12</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C34" s="9">
         <v>33</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>6</v>
@@ -5059,24 +5059,24 @@
         <v>9</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C35" s="9">
         <v>34</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F35" s="18" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G35" s="9" t="s">
         <v>6</v>
@@ -5085,24 +5085,24 @@
         <v>1</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C36" s="9">
         <v>35</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F36" s="18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>6</v>
@@ -5111,24 +5111,24 @@
         <v>2</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C37" s="9">
         <v>36</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F37" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G37" s="9" t="s">
         <v>6</v>
@@ -5137,848 +5137,848 @@
         <v>4</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C38" s="9">
         <v>37</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G38" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H38" s="8">
         <v>1</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K38" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C39" s="9">
         <v>38</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F39" s="18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H39" s="8">
         <v>1</v>
       </c>
       <c r="I39" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K39" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C40" s="9">
         <v>39</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F40" s="18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H40" s="8">
         <v>3</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K40" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C41" s="9">
         <v>40</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H41" s="8">
         <v>1</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K41" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C42" s="9">
         <v>41</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G42" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H42" s="8">
         <v>1</v>
       </c>
       <c r="K42" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C43" s="9">
         <v>42</v>
       </c>
       <c r="E43" s="18" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F43" s="18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G43" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H43" s="8">
         <v>1</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K43" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C44" s="9">
         <v>43</v>
       </c>
       <c r="E44" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="F44" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="F44" s="18" t="s">
-        <v>191</v>
-      </c>
       <c r="G44" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H44" s="8">
         <v>1</v>
       </c>
       <c r="K44" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C45" s="9">
         <v>44</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F45" s="18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G45" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H45" s="8">
         <v>1</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K45" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C46" s="9">
         <v>45</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H46" s="8">
         <v>1</v>
       </c>
       <c r="K46" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C47" s="9">
         <v>46</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H47" s="8">
         <v>1</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K47" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C48" s="9">
         <v>47</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F48" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G48" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H48" s="8">
         <v>1</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K48" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C49" s="9">
         <v>48</v>
       </c>
       <c r="E49" s="18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F49" s="18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H49" s="8">
         <v>1</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K49" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L49" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C50" s="9">
         <v>49</v>
       </c>
       <c r="E50" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F50" s="18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G50" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H50" s="8">
         <v>3</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K50" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L50" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C51" s="9">
         <v>50</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F51" s="18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G51" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H51" s="8">
         <v>1</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K51" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L51" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C52" s="9">
         <v>51</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F52" s="18" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G52" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H52" s="8">
         <v>2</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K52" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L52" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C53" s="9">
         <v>52</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F53" s="18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G53" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H53" s="8">
         <v>3</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K53" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C54" s="9">
         <v>53</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F54" s="18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G54" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H54" s="8">
         <v>4</v>
       </c>
       <c r="I54" s="16" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K54" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L54" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C55" s="9">
         <v>54</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F55" s="18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H55" s="8">
         <v>2</v>
       </c>
       <c r="I55" s="16" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K55" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L55" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C56" s="9">
         <v>55</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F56" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H56" s="8">
         <v>1</v>
       </c>
       <c r="I56" s="16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K56" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L56" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C57" s="9">
         <v>56</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F57" s="18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G57" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H57" s="8">
         <v>1</v>
       </c>
       <c r="I57" s="16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K57" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L57" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C58" s="9">
         <v>57</v>
       </c>
       <c r="E58" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F58" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H58" s="8">
         <v>1</v>
       </c>
       <c r="I58" s="16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K58" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L58" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C59" s="9">
         <v>58</v>
       </c>
       <c r="E59" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F59" s="18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H59" s="8">
         <v>1</v>
       </c>
       <c r="I59" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K59" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L59" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C60" s="9">
         <v>59</v>
       </c>
       <c r="E60" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F60" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H60" s="8">
         <v>1</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K60" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L60" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C61" s="9">
         <v>60</v>
       </c>
       <c r="E61" s="18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F61" s="18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H61" s="8">
         <v>1</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K61" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C62" s="9">
         <v>61</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F62" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H62" s="8">
         <v>1</v>
       </c>
       <c r="I62" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K62" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L62" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C63" s="9">
         <v>62</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F63" s="18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H63" s="8">
         <v>1</v>
       </c>
       <c r="J63" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="K63" s="21" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="L63" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Link to Spider coupling source added
</commit_message>
<xml_diff>
--- a/bom/BOM_ZR_V2.5.xlsx
+++ b/bom/BOM_ZR_V2.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A518C17F-EB1B-47AE-84E2-43FA5051285B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8246A1-8EAC-4BE0-A812-355412DDBAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="204">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -658,6 +658,9 @@
   </si>
   <si>
     <t>https://s.click.aliexpress.com/e/_A4bJ8W</t>
+  </si>
+  <si>
+    <t>https://s.click.aliexpress.com/e/_AVhQZK</t>
   </si>
 </sst>
 </file>
@@ -4107,8 +4110,8 @@
   <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I12" sqref="I12:K12"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="84.65" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4358,6 +4361,9 @@
       <c r="H8" s="8">
         <v>3</v>
       </c>
+      <c r="K8" s="22" t="s">
+        <v>203</v>
+      </c>
       <c r="L8" s="6" t="s">
         <v>19</v>
       </c>
@@ -6008,15 +6014,16 @@
     <hyperlink ref="K39" r:id="rId4" display="https://github.com/MirageC79/HevORT/tree/master/files/STL/ZR_V2.5" xr:uid="{E8CDD8F3-900B-4577-BD6C-D79B27C34BF0}"/>
     <hyperlink ref="K15" r:id="rId5" xr:uid="{138D10EF-E7F3-40F8-BEE8-5E7315C1A516}"/>
     <hyperlink ref="K12" r:id="rId6" xr:uid="{A4C611E4-5D85-433A-A900-A83BD7E3A0FB}"/>
+    <hyperlink ref="K8" r:id="rId7" xr:uid="{4353B053-904D-4DFB-A20F-01E25500B133}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId7"/>
-  <drawing r:id="rId8"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>
+  <drawing r:id="rId9"/>
   <webPublishItems count="1">
     <webPublishItem id="6083" divId="BOM_ZR_V2_6083" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_ZR_V2.5.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added more details on source for Z thrust bearing collar.
</commit_message>
<xml_diff>
--- a/bom/BOM_ZR_V2.5.xlsx
+++ b/bom/BOM_ZR_V2.5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8246A1-8EAC-4BE0-A812-355412DDBAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFBEE12-EBF4-4F22-A525-6247D041DCC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="205">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -597,9 +597,6 @@
     <t>Double Angular Contact Bearing</t>
   </si>
   <si>
-    <t>Ruland_57445K444_CLAMPING SHAFT COLLAR</t>
-  </si>
-  <si>
     <t>Shaft Collar, 10mm ID</t>
   </si>
   <si>
@@ -661,6 +658,12 @@
   </si>
   <si>
     <t>https://s.click.aliexpress.com/e/_AVhQZK</t>
+  </si>
+  <si>
+    <t>Ruland_57445K444_CLAMPING SHAFT COLLAR (MCL-10-F)</t>
+  </si>
+  <si>
+    <t>https://www.ruland.com/mcl-10-f.html</t>
   </si>
 </sst>
 </file>
@@ -824,7 +827,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -890,6 +893,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -4110,8 +4116,8 @@
   <dimension ref="A1:L63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="84.65" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4324,10 +4330,10 @@
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="F7" s="19" t="s">
         <v>182</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>183</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>6</v>
@@ -4337,7 +4343,9 @@
       </c>
       <c r="I7" s="17"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="K7" s="23" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
@@ -4362,7 +4370,7 @@
         <v>3</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>19</v>
@@ -4478,13 +4486,13 @@
         <v>3</v>
       </c>
       <c r="I12" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="K12" s="22" t="s">
         <v>201</v>
-      </c>
-      <c r="K12" s="22" t="s">
-        <v>202</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>31</v>
@@ -4501,10 +4509,10 @@
         <v>12</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>6</v>
@@ -4513,7 +4521,7 @@
         <v>3</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>34</v>
@@ -4542,7 +4550,7 @@
         <v>9</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>35</v>
@@ -4574,10 +4582,10 @@
         <v>169</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K15" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>36</v>
@@ -4623,10 +4631,10 @@
         <v>16</v>
       </c>
       <c r="E17" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="F17" s="18" t="s">
         <v>191</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>192</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>6</v>
@@ -5022,10 +5030,10 @@
         <v>31</v>
       </c>
       <c r="E32" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="F32" s="18" t="s">
         <v>189</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>190</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>6</v>
@@ -5193,7 +5201,7 @@
         <v>164</v>
       </c>
       <c r="K38" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L38" s="6" t="s">
         <v>88</v>
@@ -5228,7 +5236,7 @@
         <v>164</v>
       </c>
       <c r="K39" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L39" s="6" t="s">
         <v>91</v>
@@ -5263,7 +5271,7 @@
         <v>164</v>
       </c>
       <c r="K40" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L40" s="6" t="s">
         <v>94</v>
@@ -5295,7 +5303,7 @@
         <v>164</v>
       </c>
       <c r="K41" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L41" s="6" t="s">
         <v>97</v>
@@ -5312,10 +5320,10 @@
         <v>41</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>9</v>
@@ -5324,7 +5332,7 @@
         <v>1</v>
       </c>
       <c r="K42" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5353,7 +5361,7 @@
         <v>164</v>
       </c>
       <c r="K43" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L43" s="6" t="s">
         <v>100</v>
@@ -5370,10 +5378,10 @@
         <v>43</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>9</v>
@@ -5382,7 +5390,7 @@
         <v>1</v>
       </c>
       <c r="K44" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5396,7 +5404,7 @@
         <v>44</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F45" s="18" t="s">
         <v>177</v>
@@ -5411,7 +5419,7 @@
         <v>164</v>
       </c>
       <c r="K45" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L45" s="6" t="s">
         <v>102</v>
@@ -5428,10 +5436,10 @@
         <v>45</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>9</v>
@@ -5440,7 +5448,7 @@
         <v>1</v>
       </c>
       <c r="K46" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5469,7 +5477,7 @@
         <v>164</v>
       </c>
       <c r="K47" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L47" s="6" t="s">
         <v>105</v>
@@ -5501,7 +5509,7 @@
         <v>164</v>
       </c>
       <c r="K48" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L48" s="6" t="s">
         <v>108</v>
@@ -5533,7 +5541,7 @@
         <v>164</v>
       </c>
       <c r="K49" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L49" s="6" t="s">
         <v>111</v>
@@ -5565,7 +5573,7 @@
         <v>164</v>
       </c>
       <c r="K50" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L50" s="6" t="s">
         <v>114</v>
@@ -5597,7 +5605,7 @@
         <v>164</v>
       </c>
       <c r="K51" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L51" s="6" t="s">
         <v>119</v>
@@ -5629,7 +5637,7 @@
         <v>164</v>
       </c>
       <c r="K52" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L52" s="6" t="s">
         <v>121</v>
@@ -5661,7 +5669,7 @@
         <v>164</v>
       </c>
       <c r="K53" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L53" s="6" t="s">
         <v>124</v>
@@ -5696,7 +5704,7 @@
         <v>164</v>
       </c>
       <c r="K54" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L54" s="6" t="s">
         <v>127</v>
@@ -5731,7 +5739,7 @@
         <v>164</v>
       </c>
       <c r="K55" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L55" s="6" t="s">
         <v>130</v>
@@ -5766,7 +5774,7 @@
         <v>164</v>
       </c>
       <c r="K56" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L56" s="6" t="s">
         <v>133</v>
@@ -5801,7 +5809,7 @@
         <v>164</v>
       </c>
       <c r="K57" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L57" s="6" t="s">
         <v>136</v>
@@ -5836,7 +5844,7 @@
         <v>164</v>
       </c>
       <c r="K58" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L58" s="6" t="s">
         <v>133</v>
@@ -5871,7 +5879,7 @@
         <v>164</v>
       </c>
       <c r="K59" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L59" s="6" t="s">
         <v>140</v>
@@ -5903,7 +5911,7 @@
         <v>164</v>
       </c>
       <c r="K60" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L60" s="6" t="s">
         <v>143</v>
@@ -5935,7 +5943,7 @@
         <v>164</v>
       </c>
       <c r="K61" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -5967,7 +5975,7 @@
         <v>164</v>
       </c>
       <c r="K62" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L62" s="6" t="s">
         <v>147</v>
@@ -5999,7 +6007,7 @@
         <v>164</v>
       </c>
       <c r="K63" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L63" s="6" t="s">
         <v>150</v>
@@ -6015,15 +6023,16 @@
     <hyperlink ref="K15" r:id="rId5" xr:uid="{138D10EF-E7F3-40F8-BEE8-5E7315C1A516}"/>
     <hyperlink ref="K12" r:id="rId6" xr:uid="{A4C611E4-5D85-433A-A900-A83BD7E3A0FB}"/>
     <hyperlink ref="K8" r:id="rId7" xr:uid="{4353B053-904D-4DFB-A20F-01E25500B133}"/>
+    <hyperlink ref="K7" r:id="rId8" xr:uid="{73D4C11C-7527-4A83-86BB-963E4F5D666B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>
-  <drawing r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
+  <drawing r:id="rId10"/>
   <webPublishItems count="1">
     <webPublishItem id="6083" divId="BOM_ZR_V2_6083" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_ZR_V2.5.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Re aligned detailed parts picture
</commit_message>
<xml_diff>
--- a/bom/BOM_ZR_V2.5.xlsx
+++ b/bom/BOM_ZR_V2.5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DFBEE12-EBF4-4F22-A525-6247D041DCC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2C09D0-9C1C-4112-90E2-BCF028291E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1040,15 +1040,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>212727</xdr:colOff>
+      <xdr:colOff>340673</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1122802</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1071,28 +1071,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3498852" y="13500100"/>
-          <a:ext cx="975212" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3806152" y="14889668"/>
+          <a:ext cx="782129" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1115,28 +1115,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="17357725"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="18750333"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1159,28 +1159,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="3213100"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="3307674"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1203,28 +1203,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="7070725"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="8455227"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1247,28 +1247,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="59791600"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="67652089"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1291,28 +1291,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="34074100"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="36766769"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1335,28 +1335,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="26358850"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="29045440"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1379,28 +1379,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="31502350"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="34192993"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1423,28 +1423,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="27644725"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="30332328"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1467,28 +1467,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="35359975"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="38053658"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1511,28 +1511,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="50790475"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="58643870"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1555,28 +1555,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="32788225"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="35479881"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1599,28 +1599,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="39217600"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="43201211"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1643,28 +1643,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="21215350"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="23897886"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1687,28 +1687,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="45646975"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="49635652"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1731,28 +1731,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="52076350"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="59930759"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1775,28 +1775,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="40503475"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="44488099"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1819,28 +1819,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="53362225"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="61217647"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1863,28 +1863,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="61077475"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="68938977"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1907,28 +1907,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="57219850"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="65078312"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1951,28 +1951,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="18643600"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="21324110"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1995,28 +1995,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="58505725"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="66365200"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2039,28 +2039,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="19929475"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="22610998"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2083,28 +2083,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="37931725"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="41914323"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2127,28 +2127,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="14785975"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="16176557"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2171,28 +2171,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="16071850"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="17463445"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2215,28 +2215,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="55933975"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="63791424"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2259,28 +2259,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="10928350"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="12315892"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2303,28 +2303,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="641350"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="733897"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2347,28 +2347,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="70078600"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="77947195"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2391,28 +2391,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="1927225"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="2020785"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2435,28 +2435,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="41789350"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="45774987"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2479,28 +2479,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="28930600"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="31619216"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2523,28 +2523,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="67506850"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="75373418"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2567,28 +2567,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="54648100"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="62504535"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2611,28 +2611,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="36645850"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="40627434"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2655,28 +2655,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="8356600"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="9742115"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2699,28 +2699,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="12214225"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="13602780"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2743,28 +2743,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="22501225"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="25184775"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2787,28 +2787,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="66220975"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="74086530"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2831,28 +2831,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="68792725"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="76660307"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2875,28 +2875,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="71364475"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="79234083"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2919,28 +2919,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="44361100"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="48348764"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2963,28 +2963,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="43075225"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="47061876"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3007,28 +3007,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="23787100"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="26471663"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3051,28 +3051,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="9642475"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="11029003"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3095,28 +3095,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="25072975"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="27758551"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3139,28 +3139,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="30216475"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="32906105"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3183,28 +3183,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="62363350"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="70225865"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3227,28 +3227,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="4498975"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="4594562"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3271,28 +3271,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="63649225"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>209552</xdr:colOff>
+          <a:off x="3796627" y="71512753"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>331148</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1187939</xdr:colOff>
+      <xdr:rowOff>288046</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1121586</xdr:colOff>
       <xdr:row>57</xdr:row>
-      <xdr:rowOff>1135888</xdr:rowOff>
+      <xdr:rowOff>1045318</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3315,28 +3315,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3495677" y="64935100"/>
-          <a:ext cx="978387" cy="932688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>101330</xdr:colOff>
+          <a:off x="3796627" y="72799642"/>
+          <a:ext cx="790438" cy="757272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>229276</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>67553</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1285605</xdr:colOff>
+      <xdr:rowOff>158749</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1180437</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>1196512</xdr:rowOff>
+      <xdr:rowOff>1071536</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3359,28 +3359,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3546543" y="49286808"/>
-          <a:ext cx="1184275" cy="1128959"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>128351</xdr:colOff>
+          <a:off x="3694755" y="55940797"/>
+          <a:ext cx="951161" cy="912787"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>243597</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>81064</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1297544</xdr:colOff>
+      <xdr:rowOff>178610</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1197831</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>1197479</xdr:rowOff>
+      <xdr:rowOff>1072338</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3403,28 +3403,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3573564" y="48016809"/>
-          <a:ext cx="1169193" cy="1116415"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>148617</xdr:colOff>
+          <a:off x="3709076" y="53386881"/>
+          <a:ext cx="954234" cy="893728"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>263863</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>81063</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1332892</xdr:colOff>
+      <xdr:rowOff>178609</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1227116</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>1210022</xdr:rowOff>
+      <xdr:rowOff>1083087</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3447,28 +3447,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3593830" y="46733297"/>
-          <a:ext cx="1184275" cy="1128959"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>148617</xdr:colOff>
+          <a:off x="3729342" y="50813104"/>
+          <a:ext cx="963253" cy="904478"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>263863</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>87819</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1332892</xdr:colOff>
+      <xdr:rowOff>179015</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1227116</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>1216778</xdr:rowOff>
+      <xdr:rowOff>1094369</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3491,28 +3491,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3593830" y="5667713"/>
-          <a:ext cx="1184275" cy="1128959"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>114840</xdr:colOff>
+          <a:off x="3729342" y="5772419"/>
+          <a:ext cx="963253" cy="915354"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>236436</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>74308</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1299115</xdr:colOff>
+      <xdr:rowOff>165504</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1199689</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>1203267</xdr:rowOff>
+      <xdr:rowOff>1075116</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3535,28 +3535,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3560053" y="6937712"/>
-          <a:ext cx="1184275" cy="1128959"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>128351</xdr:colOff>
+          <a:off x="3701915" y="7045797"/>
+          <a:ext cx="963253" cy="909612"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>243597</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>81064</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1312626</xdr:colOff>
+      <xdr:rowOff>178610</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1206850</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>1210023</xdr:rowOff>
+      <xdr:rowOff>1083088</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3579,28 +3579,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3573564" y="51867341"/>
-          <a:ext cx="1184275" cy="1128959"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>108086</xdr:colOff>
+          <a:off x="3709076" y="57247546"/>
+          <a:ext cx="963253" cy="904478"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>223332</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>60798</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1292361</xdr:colOff>
+      <xdr:rowOff>158344</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1186585</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>1189757</xdr:rowOff>
+      <xdr:rowOff>1071131</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3623,28 +3623,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3553299" y="49280053"/>
-          <a:ext cx="1184275" cy="1128959"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>128351</xdr:colOff>
+          <a:off x="3688811" y="52079727"/>
+          <a:ext cx="963253" cy="912787"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>243597</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>81064</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1297544</xdr:colOff>
+      <xdr:rowOff>178610</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1197831</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>1197479</xdr:rowOff>
+      <xdr:rowOff>1072338</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3667,28 +3667,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3573564" y="51867341"/>
-          <a:ext cx="1169193" cy="1116415"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>128351</xdr:colOff>
+          <a:off x="3709076" y="54673770"/>
+          <a:ext cx="954234" cy="893728"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>243597</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>67553</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1312626</xdr:colOff>
+      <xdr:rowOff>158749</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1206850</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>1196512</xdr:rowOff>
+      <xdr:rowOff>1071536</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3711,28 +3711,28 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3573564" y="37735213"/>
-          <a:ext cx="1184275" cy="1128959"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>108085</xdr:colOff>
+          <a:off x="3709076" y="39211249"/>
+          <a:ext cx="963253" cy="912787"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>223331</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>87819</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1292360</xdr:colOff>
+      <xdr:rowOff>179015</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1186584</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1216778</xdr:rowOff>
+      <xdr:rowOff>1094369</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3755,8 +3755,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3553298" y="19786330"/>
-          <a:ext cx="1184275" cy="1128959"/>
+          <a:off x="3688810" y="19928191"/>
+          <a:ext cx="963253" cy="915354"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4115,9 +4115,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="84.65" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Notes added for 22mm Dia SFU1204
</commit_message>
<xml_diff>
--- a/bom/BOM_ZR_V2.5.xlsx
+++ b/bom/BOM_ZR_V2.5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A7652E-9FD7-4396-81EA-F7FA94DFA432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CD381F-A85F-4430-BCEE-0BF0B021A4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="207">
   <si>
     <t>Thumbnail</t>
   </si>
@@ -576,9 +576,6 @@
     <t>Commonly available (same springs as most printers)</t>
   </si>
   <si>
-    <t>BK10 and BF10 machined end required.   BK10 and BF10 blocks ARE NOT required.</t>
-  </si>
-  <si>
     <t>ZR_MotorMount_RR_Body_V2.5</t>
   </si>
   <si>
@@ -664,13 +661,47 @@
   </si>
   <si>
     <t>https://www.ruland.com/mcl-10-f.html</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">BK10 and BF10 machined end required.   BK10 and BF10 blocks ARE NOT required.  Length 450mm fits Z axis of 340mm.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*Nut cylindrical portion should have a diamerter of 22mm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Length determined by Frame Calculator:
+https://github.com/MirageC79/HevORT/tree/master/docs/assets/references/frame</t>
+    </r>
+  </si>
+  <si>
+    <t>AliExpress</t>
+  </si>
+  <si>
+    <t>https://s.click.aliexpress.com/e/_DdCsRNX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -764,6 +795,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -827,7 +872,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -897,6 +942,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4117,7 +4168,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="84.65" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4177,7 +4228,7 @@
     </row>
     <row r="2" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>6</v>
@@ -4206,7 +4257,7 @@
     </row>
     <row r="3" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>6</v>
@@ -4233,9 +4284,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="124" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>6</v>
@@ -4255,8 +4306,14 @@
       <c r="H4" s="8">
         <v>3</v>
       </c>
-      <c r="I4" s="20" t="s">
-        <v>175</v>
+      <c r="I4" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>206</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>10</v>
@@ -4264,7 +4321,7 @@
     </row>
     <row r="5" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>6</v>
@@ -4290,7 +4347,7 @@
     </row>
     <row r="6" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>6</v>
@@ -4300,10 +4357,10 @@
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>180</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>181</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>6</v>
@@ -4320,7 +4377,7 @@
     </row>
     <row r="7" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>6</v>
@@ -4330,10 +4387,10 @@
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G7" s="11" t="s">
         <v>6</v>
@@ -4344,12 +4401,12 @@
       <c r="I7" s="17"/>
       <c r="J7" s="10"/>
       <c r="K7" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>6</v>
@@ -4370,7 +4427,7 @@
         <v>3</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>19</v>
@@ -4378,7 +4435,7 @@
     </row>
     <row r="9" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>6</v>
@@ -4404,7 +4461,7 @@
     </row>
     <row r="10" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>6</v>
@@ -4433,7 +4490,7 @@
     </row>
     <row r="11" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>6</v>
@@ -4465,7 +4522,7 @@
     </row>
     <row r="12" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>6</v>
@@ -4486,13 +4543,13 @@
         <v>3</v>
       </c>
       <c r="I12" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="J12" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="K12" s="22" t="s">
         <v>200</v>
-      </c>
-      <c r="K12" s="22" t="s">
-        <v>201</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>31</v>
@@ -4500,7 +4557,7 @@
     </row>
     <row r="13" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>6</v>
@@ -4509,10 +4566,10 @@
         <v>12</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>6</v>
@@ -4521,7 +4578,7 @@
         <v>3</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>34</v>
@@ -4529,7 +4586,7 @@
     </row>
     <row r="14" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>157</v>
@@ -4550,7 +4607,7 @@
         <v>9</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L14" s="6" t="s">
         <v>35</v>
@@ -4558,7 +4615,7 @@
     </row>
     <row r="15" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>157</v>
@@ -4582,10 +4639,10 @@
         <v>169</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K15" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L15" s="6" t="s">
         <v>36</v>
@@ -4593,7 +4650,7 @@
     </row>
     <row r="16" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>157</v>
@@ -4622,7 +4679,7 @@
     </row>
     <row r="17" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>157</v>
@@ -4631,10 +4688,10 @@
         <v>16</v>
       </c>
       <c r="E17" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="F17" s="18" t="s">
         <v>190</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>191</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>6</v>
@@ -4645,7 +4702,7 @@
     </row>
     <row r="18" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>157</v>
@@ -4671,7 +4728,7 @@
     </row>
     <row r="19" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>157</v>
@@ -4697,7 +4754,7 @@
     </row>
     <row r="20" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>157</v>
@@ -4723,7 +4780,7 @@
     </row>
     <row r="21" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B21" s="14" t="s">
         <v>157</v>
@@ -4752,7 +4809,7 @@
     </row>
     <row r="22" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>157</v>
@@ -4781,7 +4838,7 @@
     </row>
     <row r="23" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>157</v>
@@ -4810,7 +4867,7 @@
     </row>
     <row r="24" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>157</v>
@@ -4839,7 +4896,7 @@
     </row>
     <row r="25" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>157</v>
@@ -4865,7 +4922,7 @@
     </row>
     <row r="26" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B26" s="14" t="s">
         <v>157</v>
@@ -4891,7 +4948,7 @@
     </row>
     <row r="27" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>157</v>
@@ -4917,7 +4974,7 @@
     </row>
     <row r="28" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B28" s="14" t="s">
         <v>157</v>
@@ -4943,7 +5000,7 @@
     </row>
     <row r="29" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B29" s="14" t="s">
         <v>157</v>
@@ -4969,7 +5026,7 @@
     </row>
     <row r="30" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>157</v>
@@ -4995,7 +5052,7 @@
     </row>
     <row r="31" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B31" s="14" t="s">
         <v>157</v>
@@ -5021,7 +5078,7 @@
     </row>
     <row r="32" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B32" s="14" t="s">
         <v>157</v>
@@ -5030,10 +5087,10 @@
         <v>31</v>
       </c>
       <c r="E32" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="F32" s="18" t="s">
         <v>188</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>189</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>6</v>
@@ -5044,7 +5101,7 @@
     </row>
     <row r="33" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B33" s="14" t="s">
         <v>157</v>
@@ -5070,7 +5127,7 @@
     </row>
     <row r="34" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>157</v>
@@ -5096,7 +5153,7 @@
     </row>
     <row r="35" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B35" s="14" t="s">
         <v>157</v>
@@ -5122,7 +5179,7 @@
     </row>
     <row r="36" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>157</v>
@@ -5148,7 +5205,7 @@
     </row>
     <row r="37" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B37" s="14" t="s">
         <v>157</v>
@@ -5174,7 +5231,7 @@
     </row>
     <row r="38" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B38" s="14" t="s">
         <v>9</v>
@@ -5201,7 +5258,7 @@
         <v>164</v>
       </c>
       <c r="K38" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L38" s="6" t="s">
         <v>88</v>
@@ -5209,7 +5266,7 @@
     </row>
     <row r="39" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B39" s="14" t="s">
         <v>9</v>
@@ -5236,7 +5293,7 @@
         <v>164</v>
       </c>
       <c r="K39" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L39" s="6" t="s">
         <v>91</v>
@@ -5244,7 +5301,7 @@
     </row>
     <row r="40" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B40" s="14" t="s">
         <v>9</v>
@@ -5271,7 +5328,7 @@
         <v>164</v>
       </c>
       <c r="K40" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L40" s="6" t="s">
         <v>94</v>
@@ -5279,7 +5336,7 @@
     </row>
     <row r="41" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B41" s="14" t="s">
         <v>9</v>
@@ -5288,10 +5345,10 @@
         <v>40</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G41" s="9" t="s">
         <v>9</v>
@@ -5303,7 +5360,7 @@
         <v>164</v>
       </c>
       <c r="K41" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L41" s="6" t="s">
         <v>97</v>
@@ -5311,7 +5368,7 @@
     </row>
     <row r="42" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B42" s="14" t="s">
         <v>9</v>
@@ -5320,10 +5377,10 @@
         <v>41</v>
       </c>
       <c r="E42" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F42" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>9</v>
@@ -5332,12 +5389,12 @@
         <v>1</v>
       </c>
       <c r="K42" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B43" s="14" t="s">
         <v>9</v>
@@ -5346,10 +5403,10 @@
         <v>42</v>
       </c>
       <c r="E43" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="F43" s="18" t="s">
         <v>176</v>
-      </c>
-      <c r="F43" s="18" t="s">
-        <v>177</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>9</v>
@@ -5361,7 +5418,7 @@
         <v>164</v>
       </c>
       <c r="K43" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L43" s="6" t="s">
         <v>100</v>
@@ -5369,7 +5426,7 @@
     </row>
     <row r="44" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B44" s="14" t="s">
         <v>9</v>
@@ -5378,10 +5435,10 @@
         <v>43</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>9</v>
@@ -5390,12 +5447,12 @@
         <v>1</v>
       </c>
       <c r="K44" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>9</v>
@@ -5404,10 +5461,10 @@
         <v>44</v>
       </c>
       <c r="E45" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F45" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>9</v>
@@ -5419,7 +5476,7 @@
         <v>164</v>
       </c>
       <c r="K45" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L45" s="6" t="s">
         <v>102</v>
@@ -5427,7 +5484,7 @@
     </row>
     <row r="46" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>9</v>
@@ -5436,10 +5493,10 @@
         <v>45</v>
       </c>
       <c r="E46" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F46" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>9</v>
@@ -5448,12 +5505,12 @@
         <v>1</v>
       </c>
       <c r="K46" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B47" s="14" t="s">
         <v>9</v>
@@ -5477,7 +5534,7 @@
         <v>164</v>
       </c>
       <c r="K47" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L47" s="6" t="s">
         <v>105</v>
@@ -5485,7 +5542,7 @@
     </row>
     <row r="48" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B48" s="14" t="s">
         <v>9</v>
@@ -5509,7 +5566,7 @@
         <v>164</v>
       </c>
       <c r="K48" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L48" s="6" t="s">
         <v>108</v>
@@ -5517,7 +5574,7 @@
     </row>
     <row r="49" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B49" s="14" t="s">
         <v>9</v>
@@ -5541,7 +5598,7 @@
         <v>164</v>
       </c>
       <c r="K49" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L49" s="6" t="s">
         <v>111</v>
@@ -5549,7 +5606,7 @@
     </row>
     <row r="50" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B50" s="14" t="s">
         <v>9</v>
@@ -5573,7 +5630,7 @@
         <v>164</v>
       </c>
       <c r="K50" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L50" s="6" t="s">
         <v>114</v>
@@ -5581,7 +5638,7 @@
     </row>
     <row r="51" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B51" s="14" t="s">
         <v>9</v>
@@ -5605,7 +5662,7 @@
         <v>164</v>
       </c>
       <c r="K51" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L51" s="6" t="s">
         <v>119</v>
@@ -5613,7 +5670,7 @@
     </row>
     <row r="52" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B52" s="14" t="s">
         <v>9</v>
@@ -5637,7 +5694,7 @@
         <v>164</v>
       </c>
       <c r="K52" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L52" s="6" t="s">
         <v>121</v>
@@ -5645,7 +5702,7 @@
     </row>
     <row r="53" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>9</v>
@@ -5669,7 +5726,7 @@
         <v>164</v>
       </c>
       <c r="K53" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L53" s="6" t="s">
         <v>124</v>
@@ -5677,7 +5734,7 @@
     </row>
     <row r="54" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B54" s="14" t="s">
         <v>9</v>
@@ -5704,7 +5761,7 @@
         <v>164</v>
       </c>
       <c r="K54" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L54" s="6" t="s">
         <v>127</v>
@@ -5712,7 +5769,7 @@
     </row>
     <row r="55" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B55" s="14" t="s">
         <v>9</v>
@@ -5739,7 +5796,7 @@
         <v>164</v>
       </c>
       <c r="K55" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L55" s="6" t="s">
         <v>130</v>
@@ -5747,7 +5804,7 @@
     </row>
     <row r="56" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>9</v>
@@ -5774,7 +5831,7 @@
         <v>164</v>
       </c>
       <c r="K56" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L56" s="6" t="s">
         <v>133</v>
@@ -5782,7 +5839,7 @@
     </row>
     <row r="57" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B57" s="14" t="s">
         <v>9</v>
@@ -5809,7 +5866,7 @@
         <v>164</v>
       </c>
       <c r="K57" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L57" s="6" t="s">
         <v>136</v>
@@ -5817,7 +5874,7 @@
     </row>
     <row r="58" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B58" s="14" t="s">
         <v>9</v>
@@ -5844,7 +5901,7 @@
         <v>164</v>
       </c>
       <c r="K58" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L58" s="6" t="s">
         <v>133</v>
@@ -5852,7 +5909,7 @@
     </row>
     <row r="59" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B59" s="14" t="s">
         <v>9</v>
@@ -5879,7 +5936,7 @@
         <v>164</v>
       </c>
       <c r="K59" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L59" s="6" t="s">
         <v>140</v>
@@ -5887,7 +5944,7 @@
     </row>
     <row r="60" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B60" s="14" t="s">
         <v>9</v>
@@ -5911,7 +5968,7 @@
         <v>164</v>
       </c>
       <c r="K60" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L60" s="6" t="s">
         <v>143</v>
@@ -5919,7 +5976,7 @@
     </row>
     <row r="61" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B61" s="14" t="s">
         <v>9</v>
@@ -5943,12 +6000,12 @@
         <v>164</v>
       </c>
       <c r="K61" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B62" s="14" t="s">
         <v>9</v>
@@ -5975,7 +6032,7 @@
         <v>164</v>
       </c>
       <c r="K62" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L62" s="6" t="s">
         <v>147</v>
@@ -5983,7 +6040,7 @@
     </row>
     <row r="63" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B63" s="14" t="s">
         <v>9</v>
@@ -6007,7 +6064,7 @@
         <v>164</v>
       </c>
       <c r="K63" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L63" s="6" t="s">
         <v>150</v>
@@ -6024,15 +6081,16 @@
     <hyperlink ref="K12" r:id="rId6" xr:uid="{A4C611E4-5D85-433A-A900-A83BD7E3A0FB}"/>
     <hyperlink ref="K8" r:id="rId7" xr:uid="{4353B053-904D-4DFB-A20F-01E25500B133}"/>
     <hyperlink ref="K7" r:id="rId8" xr:uid="{73D4C11C-7527-4A83-86BB-963E4F5D666B}"/>
+    <hyperlink ref="K4" r:id="rId9" xr:uid="{B82770E7-12B2-498B-9A21-5DAF92DCFBA8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId9"/>
-  <drawing r:id="rId10"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId10"/>
+  <drawing r:id="rId11"/>
   <webPublishItems count="1">
     <webPublishItem id="6083" divId="BOM_ZR_V2_6083" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_ZR_V2.5.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
SFU1204 nut diameter Issue 43 clarification
https://github.com/MirageC79/HevORT/issues/43
</commit_message>
<xml_diff>
--- a/bom/BOM_ZR_V2.5.xlsx
+++ b/bom/BOM_ZR_V2.5.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CD381F-A85F-4430-BCEE-0BF0B021A4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207F559B-4547-4C15-8278-B370C259FF72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,12 +74,6 @@
     <t>d901dba6ddbd4127bf0567ea10fe573a</t>
   </si>
   <si>
-    <t>SFU1204-450 With Nut</t>
-  </si>
-  <si>
-    <t>BAll Screw with Nut</t>
-  </si>
-  <si>
     <t>de33ba5276229899d11c6192b196a71f</t>
   </si>
   <si>
@@ -663,6 +657,19 @@
     <t>https://www.ruland.com/mcl-10-f.html</t>
   </si>
   <si>
+    <t>AliExpress</t>
+  </si>
+  <si>
+    <t>https://s.click.aliexpress.com/e/_DdCsRNX</t>
+  </si>
+  <si>
+    <t>SFU1204-450(-3)* With Nut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ball Screw with 22mm diameter Nut
+ </t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">BK10 and BF10 machined end required.   BK10 and BF10 blocks ARE NOT required.  Length 450mm fits Z axis of 340mm.
 </t>
@@ -675,7 +682,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>*Nut cylindrical portion should have a diamerter of 22mm</t>
+      <t>*Nut cylindrical portion should have a diamerter of 22mm
+Some supplier will Identify as -3.</t>
     </r>
     <r>
       <rPr>
@@ -689,12 +697,6 @@
 Length determined by Frame Calculator:
 https://github.com/MirageC79/HevORT/tree/master/docs/assets/references/frame</t>
     </r>
-  </si>
-  <si>
-    <t>AliExpress</t>
-  </si>
-  <si>
-    <t>https://s.click.aliexpress.com/e/_DdCsRNX</t>
   </si>
 </sst>
 </file>
@@ -872,7 +874,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -901,37 +903,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -948,6 +929,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3844,9 +3828,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3884,9 +3868,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3919,26 +3903,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3971,26 +3938,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4166,22 +4116,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="84.65" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.453125" style="13"/>
-    <col min="2" max="2" width="16.453125" style="14"/>
+    <col min="1" max="1" width="16.453125" style="10"/>
+    <col min="2" max="2" width="16.453125" style="11"/>
     <col min="3" max="3" width="16.453125" style="9"/>
     <col min="4" max="4" width="20.7265625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="44.81640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="49" style="18" customWidth="1"/>
+    <col min="5" max="5" width="44.81640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49" style="13" customWidth="1"/>
     <col min="7" max="7" width="14.81640625" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.453125" style="8"/>
-    <col min="9" max="9" width="56.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="56.1796875" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.453125" style="6"/>
     <col min="11" max="11" width="39.81640625" style="6" customWidth="1"/>
     <col min="12" max="12" width="33.81640625" style="6" hidden="1" customWidth="1"/>
@@ -4190,13 +4140,13 @@
   <sheetData>
     <row r="1" spans="1:12" ht="35.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
@@ -4205,16 +4155,16 @@
         <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>3</v>
@@ -4227,20 +4177,20 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B2" s="14" t="s">
+      <c r="A2" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
       </c>
-      <c r="E2" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>87</v>
+      <c r="E2" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>85</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>6</v>
@@ -4248,28 +4198,28 @@
       <c r="H2" s="8">
         <v>1</v>
       </c>
-      <c r="I2" s="16" t="s">
-        <v>160</v>
+      <c r="I2" s="12" t="s">
+        <v>158</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="9">
         <v>2</v>
       </c>
-      <c r="E3" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>93</v>
+      <c r="E3" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>6</v>
@@ -4277,28 +4227,28 @@
       <c r="H3" s="8">
         <v>4</v>
       </c>
-      <c r="I3" s="20" t="s">
-        <v>174</v>
+      <c r="I3" s="12" t="s">
+        <v>172</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="124" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B4" s="14" t="s">
+    <row r="4" spans="1:12" ht="139.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="9">
         <v>3</v>
       </c>
-      <c r="E4" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>15</v>
+      <c r="E4" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>205</v>
       </c>
       <c r="G4" s="9" t="s">
         <v>6</v>
@@ -4306,34 +4256,34 @@
       <c r="H4" s="8">
         <v>3</v>
       </c>
-      <c r="I4" s="24" t="s">
-        <v>204</v>
-      </c>
-      <c r="J4" s="25" t="s">
-        <v>205</v>
-      </c>
-      <c r="K4" s="21" t="s">
+      <c r="I4" s="17" t="s">
         <v>206</v>
+      </c>
+      <c r="J4" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>203</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B5" s="14" t="s">
+      <c r="A5" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="9">
         <v>4</v>
       </c>
-      <c r="E5" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>159</v>
+      <c r="E5" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>157</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>6</v>
@@ -4346,79 +4296,72 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="9">
         <v>5</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="G6" s="11" t="s">
+      <c r="E6" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="8">
         <v>3</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
       <c r="L6" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="9">
         <v>6</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="G7" s="11" t="s">
+      <c r="E7" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="8">
         <v>3</v>
       </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="23" t="s">
-        <v>203</v>
+      <c r="K7" s="16" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B8" s="14" t="s">
+      <c r="A8" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="9">
         <v>7</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>18</v>
+      <c r="E8" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>6</v>
@@ -4426,28 +4369,28 @@
       <c r="H8" s="8">
         <v>3</v>
       </c>
-      <c r="K8" s="22" t="s">
-        <v>201</v>
+      <c r="K8" s="15" t="s">
+        <v>199</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B9" s="14" t="s">
+      <c r="A9" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="9">
         <v>8</v>
       </c>
-      <c r="E9" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>110</v>
+      <c r="E9" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>6</v>
@@ -4456,24 +4399,24 @@
         <v>3</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B10" s="14" t="s">
+      <c r="A10" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="9">
         <v>9</v>
       </c>
-      <c r="E10" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>135</v>
+      <c r="E10" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>133</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>6</v>
@@ -4481,28 +4424,28 @@
       <c r="H10" s="8">
         <v>3</v>
       </c>
-      <c r="I10" s="16" t="s">
-        <v>160</v>
+      <c r="I10" s="12" t="s">
+        <v>158</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="9">
         <v>10</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>84</v>
+      <c r="E11" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>6</v>
@@ -4510,31 +4453,31 @@
       <c r="H11" s="8">
         <v>1</v>
       </c>
-      <c r="I11" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>173</v>
+      <c r="I11" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>171</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B12" s="14" t="s">
+      <c r="A12" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="9">
         <v>11</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>113</v>
+      <c r="E12" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>6</v>
@@ -4542,34 +4485,34 @@
       <c r="H12" s="8">
         <v>3</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="I12" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="K12" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="J12" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="K12" s="22" t="s">
-        <v>200</v>
-      </c>
       <c r="L12" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B13" s="14" t="s">
+      <c r="A13" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="9">
         <v>12</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="F13" s="13" t="s">
         <v>195</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>197</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>6</v>
@@ -4577,28 +4520,28 @@
       <c r="H13" s="8">
         <v>3</v>
       </c>
-      <c r="I13" s="16" t="s">
-        <v>196</v>
+      <c r="I13" s="12" t="s">
+        <v>194</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>157</v>
+      <c r="A14" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C14" s="9">
         <v>13</v>
       </c>
-      <c r="E14" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>79</v>
+      <c r="E14" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>77</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>6</v>
@@ -4606,28 +4549,28 @@
       <c r="H14" s="8">
         <v>9</v>
       </c>
-      <c r="I14" s="20" t="s">
-        <v>191</v>
+      <c r="I14" s="12" t="s">
+        <v>189</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>157</v>
+      <c r="A15" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C15" s="9">
         <v>14</v>
       </c>
-      <c r="E15" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>168</v>
+      <c r="E15" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>166</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>6</v>
@@ -4635,33 +4578,33 @@
       <c r="H15" s="8">
         <v>30</v>
       </c>
-      <c r="I15" s="16" t="s">
-        <v>169</v>
+      <c r="I15" s="12" t="s">
+        <v>167</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="K15" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>191</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>157</v>
+      <c r="A16" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C16" s="9">
         <v>15</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="13" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="9" t="s">
@@ -4670,28 +4613,28 @@
       <c r="H16" s="8">
         <v>3</v>
       </c>
-      <c r="I16" s="16" t="s">
-        <v>161</v>
+      <c r="I16" s="12" t="s">
+        <v>159</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>157</v>
+      <c r="A17" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C17" s="9">
         <v>16</v>
       </c>
-      <c r="E17" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>190</v>
+      <c r="E17" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>188</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>6</v>
@@ -4701,20 +4644,20 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>157</v>
+      <c r="A18" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C18" s="9">
         <v>17</v>
       </c>
-      <c r="E18" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="18" t="s">
-        <v>68</v>
+      <c r="E18" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="G18" s="9" t="s">
         <v>6</v>
@@ -4723,24 +4666,24 @@
         <v>22</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>157</v>
+      <c r="A19" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C19" s="9">
         <v>18</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>73</v>
+      <c r="E19" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>71</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>6</v>
@@ -4749,24 +4692,24 @@
         <v>9</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>157</v>
+      <c r="A20" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C20" s="9">
         <v>19</v>
       </c>
-      <c r="E20" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>50</v>
+      <c r="E20" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="G20" s="9" t="s">
         <v>6</v>
@@ -4775,24 +4718,24 @@
         <v>6</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>157</v>
+      <c r="A21" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C21" s="9">
         <v>20</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>115</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>116</v>
+      <c r="E21" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>6</v>
@@ -4800,28 +4743,28 @@
       <c r="H21" s="8">
         <v>26</v>
       </c>
-      <c r="I21" s="16" t="s">
-        <v>162</v>
+      <c r="I21" s="12" t="s">
+        <v>160</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B22" s="14" t="s">
-        <v>157</v>
+      <c r="A22" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C22" s="9">
         <v>21</v>
       </c>
-      <c r="E22" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>171</v>
+      <c r="E22" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>169</v>
       </c>
       <c r="G22" s="9" t="s">
         <v>6</v>
@@ -4829,28 +4772,28 @@
       <c r="H22" s="8">
         <v>24</v>
       </c>
-      <c r="I22" s="16" t="s">
-        <v>172</v>
+      <c r="I22" s="12" t="s">
+        <v>170</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>157</v>
+      <c r="A23" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C23" s="9">
         <v>22</v>
       </c>
-      <c r="E23" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>132</v>
+      <c r="E23" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>130</v>
       </c>
       <c r="G23" s="9" t="s">
         <v>6</v>
@@ -4858,28 +4801,28 @@
       <c r="H23" s="8">
         <v>6</v>
       </c>
-      <c r="I23" s="16" t="s">
-        <v>162</v>
+      <c r="I23" s="12" t="s">
+        <v>160</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>157</v>
+      <c r="A24" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C24" s="9">
         <v>23</v>
       </c>
-      <c r="E24" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>27</v>
+      <c r="E24" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>25</v>
       </c>
       <c r="G24" s="9" t="s">
         <v>6</v>
@@ -4887,28 +4830,28 @@
       <c r="H24" s="8">
         <v>15</v>
       </c>
-      <c r="I24" s="16" t="s">
-        <v>162</v>
+      <c r="I24" s="12" t="s">
+        <v>160</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>157</v>
+      <c r="A25" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C25" s="9">
         <v>24</v>
       </c>
-      <c r="E25" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>33</v>
+      <c r="E25" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="G25" s="9" t="s">
         <v>6</v>
@@ -4917,24 +4860,24 @@
         <v>3</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>157</v>
+      <c r="A26" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C26" s="9">
         <v>25</v>
       </c>
-      <c r="E26" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>99</v>
+      <c r="E26" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>97</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>6</v>
@@ -4943,24 +4886,24 @@
         <v>26</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>157</v>
+      <c r="A27" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C27" s="9">
         <v>26</v>
       </c>
-      <c r="E27" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="F27" s="18" t="s">
-        <v>139</v>
+      <c r="E27" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>137</v>
       </c>
       <c r="G27" s="9" t="s">
         <v>6</v>
@@ -4969,24 +4912,24 @@
         <v>6</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>157</v>
+      <c r="A28" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C28" s="9">
         <v>27</v>
       </c>
-      <c r="E28" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F28" s="18" t="s">
-        <v>30</v>
+      <c r="E28" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>28</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>6</v>
@@ -4995,24 +4938,24 @@
         <v>16</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>157</v>
+      <c r="A29" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C29" s="9">
         <v>28</v>
       </c>
-      <c r="E29" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>44</v>
+      <c r="E29" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="G29" s="9" t="s">
         <v>6</v>
@@ -5021,24 +4964,24 @@
         <v>46</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>157</v>
+      <c r="A30" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C30" s="9">
         <v>29</v>
       </c>
-      <c r="E30" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F30" s="18" t="s">
-        <v>24</v>
+      <c r="E30" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>22</v>
       </c>
       <c r="G30" s="9" t="s">
         <v>6</v>
@@ -5047,24 +4990,24 @@
         <v>18</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B31" s="14" t="s">
-        <v>157</v>
+      <c r="A31" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C31" s="9">
         <v>30</v>
       </c>
-      <c r="E31" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>38</v>
+      <c r="E31" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>36</v>
       </c>
       <c r="G31" s="9" t="s">
         <v>6</v>
@@ -5073,24 +5016,24 @@
         <v>4</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>157</v>
+      <c r="A32" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C32" s="9">
         <v>31</v>
       </c>
-      <c r="E32" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>188</v>
+      <c r="E32" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="G32" s="9" t="s">
         <v>6</v>
@@ -5100,20 +5043,20 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>157</v>
+      <c r="A33" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C33" s="9">
         <v>32</v>
       </c>
-      <c r="E33" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>107</v>
+      <c r="E33" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="G33" s="9" t="s">
         <v>6</v>
@@ -5122,24 +5065,24 @@
         <v>12</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>157</v>
+      <c r="A34" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C34" s="9">
         <v>33</v>
       </c>
-      <c r="E34" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="F34" s="18" t="s">
-        <v>76</v>
+      <c r="E34" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>74</v>
       </c>
       <c r="G34" s="9" t="s">
         <v>6</v>
@@ -5148,24 +5091,24 @@
         <v>9</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>157</v>
+      <c r="A35" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C35" s="9">
         <v>34</v>
       </c>
-      <c r="E35" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>47</v>
+      <c r="E35" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="G35" s="9" t="s">
         <v>6</v>
@@ -5174,24 +5117,24 @@
         <v>1</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>157</v>
+      <c r="A36" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C36" s="9">
         <v>35</v>
       </c>
-      <c r="E36" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>58</v>
+      <c r="E36" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>56</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>6</v>
@@ -5200,24 +5143,24 @@
         <v>2</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>157</v>
+      <c r="A37" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="C37" s="9">
         <v>36</v>
       </c>
-      <c r="E37" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>96</v>
+      <c r="E37" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="G37" s="9" t="s">
         <v>6</v>
@@ -5226,24 +5169,24 @@
         <v>4</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B38" s="14" t="s">
+      <c r="A38" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="9">
         <v>37</v>
       </c>
-      <c r="E38" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="F38" s="18" t="s">
-        <v>129</v>
+      <c r="E38" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>127</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>9</v>
@@ -5251,34 +5194,34 @@
       <c r="H38" s="8">
         <v>1</v>
       </c>
-      <c r="I38" s="16" t="s">
-        <v>166</v>
+      <c r="I38" s="12" t="s">
+        <v>164</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K38" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K38" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B39" s="14" t="s">
+      <c r="A39" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C39" s="9">
         <v>38</v>
       </c>
-      <c r="E39" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="F39" s="18" t="s">
-        <v>126</v>
+      <c r="E39" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>124</v>
       </c>
       <c r="G39" s="9" t="s">
         <v>9</v>
@@ -5286,34 +5229,34 @@
       <c r="H39" s="8">
         <v>1</v>
       </c>
-      <c r="I39" s="16" t="s">
-        <v>166</v>
+      <c r="I39" s="12" t="s">
+        <v>164</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K39" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B40" s="14" t="s">
+      <c r="A40" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B40" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C40" s="9">
         <v>39</v>
       </c>
-      <c r="E40" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="F40" s="18" t="s">
-        <v>53</v>
+      <c r="E40" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="G40" s="9" t="s">
         <v>9</v>
@@ -5321,34 +5264,34 @@
       <c r="H40" s="8">
         <v>3</v>
       </c>
-      <c r="I40" s="16" t="s">
-        <v>170</v>
+      <c r="I40" s="12" t="s">
+        <v>168</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K40" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K40" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B41" s="14" t="s">
+      <c r="A41" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="9">
         <v>40</v>
       </c>
-      <c r="E41" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="F41" s="18" t="s">
+      <c r="E41" s="13" t="s">
         <v>176</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>174</v>
       </c>
       <c r="G41" s="9" t="s">
         <v>9</v>
@@ -5357,30 +5300,30 @@
         <v>1</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K41" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K41" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B42" s="14" t="s">
+      <c r="A42" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B42" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C42" s="9">
         <v>41</v>
       </c>
-      <c r="E42" s="18" t="s">
+      <c r="E42" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="F42" s="13" t="s">
         <v>184</v>
-      </c>
-      <c r="F42" s="18" t="s">
-        <v>186</v>
       </c>
       <c r="G42" s="9" t="s">
         <v>9</v>
@@ -5388,25 +5331,25 @@
       <c r="H42" s="8">
         <v>1</v>
       </c>
-      <c r="K42" s="21" t="s">
-        <v>192</v>
+      <c r="K42" s="14" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B43" s="14" t="s">
+      <c r="A43" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B43" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C43" s="9">
         <v>42</v>
       </c>
-      <c r="E43" s="18" t="s">
-        <v>175</v>
-      </c>
-      <c r="F43" s="18" t="s">
-        <v>176</v>
+      <c r="E43" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>174</v>
       </c>
       <c r="G43" s="9" t="s">
         <v>9</v>
@@ -5415,30 +5358,30 @@
         <v>1</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K43" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K43" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B44" s="14" t="s">
+      <c r="A44" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C44" s="9">
         <v>43</v>
       </c>
-      <c r="E44" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="F44" s="18" t="s">
-        <v>186</v>
+      <c r="E44" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>9</v>
@@ -5446,25 +5389,25 @@
       <c r="H44" s="8">
         <v>1</v>
       </c>
-      <c r="K44" s="21" t="s">
-        <v>192</v>
+      <c r="K44" s="14" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B45" s="14" t="s">
+      <c r="A45" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B45" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C45" s="9">
         <v>44</v>
       </c>
-      <c r="E45" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="F45" s="18" t="s">
-        <v>176</v>
+      <c r="E45" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>174</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>9</v>
@@ -5473,30 +5416,30 @@
         <v>1</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K45" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K45" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B46" s="14" t="s">
+      <c r="A46" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B46" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C46" s="9">
         <v>45</v>
       </c>
-      <c r="E46" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="F46" s="18" t="s">
-        <v>186</v>
+      <c r="E46" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>184</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>9</v>
@@ -5504,25 +5447,25 @@
       <c r="H46" s="8">
         <v>1</v>
       </c>
-      <c r="K46" s="21" t="s">
-        <v>192</v>
+      <c r="K46" s="14" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B47" s="14" t="s">
+      <c r="A47" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B47" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C47" s="9">
         <v>46</v>
       </c>
-      <c r="E47" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F47" s="18" t="s">
-        <v>41</v>
+      <c r="E47" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="G47" s="9" t="s">
         <v>9</v>
@@ -5531,30 +5474,30 @@
         <v>1</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K47" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K47" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B48" s="14" t="s">
+      <c r="A48" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B48" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C48" s="9">
         <v>47</v>
       </c>
-      <c r="E48" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F48" s="18" t="s">
-        <v>41</v>
+      <c r="E48" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>9</v>
@@ -5563,30 +5506,30 @@
         <v>1</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K48" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K48" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B49" s="14" t="s">
+      <c r="A49" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B49" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C49" s="9">
         <v>48</v>
       </c>
-      <c r="E49" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="F49" s="18" t="s">
-        <v>41</v>
+      <c r="E49" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="G49" s="9" t="s">
         <v>9</v>
@@ -5595,30 +5538,30 @@
         <v>1</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K49" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K49" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L49" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B50" s="14" t="s">
+      <c r="A50" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B50" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C50" s="9">
         <v>49</v>
       </c>
-      <c r="E50" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="F50" s="18" t="s">
-        <v>104</v>
+      <c r="E50" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F50" s="13" t="s">
+        <v>102</v>
       </c>
       <c r="G50" s="9" t="s">
         <v>9</v>
@@ -5627,30 +5570,30 @@
         <v>3</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K50" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K50" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L50" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B51" s="14" t="s">
+      <c r="A51" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B51" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C51" s="9">
         <v>50</v>
       </c>
-      <c r="E51" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="F51" s="18" t="s">
-        <v>82</v>
+      <c r="E51" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F51" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="G51" s="9" t="s">
         <v>9</v>
@@ -5659,30 +5602,30 @@
         <v>1</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K51" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K51" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L51" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B52" s="14" t="s">
+      <c r="A52" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B52" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C52" s="9">
         <v>51</v>
       </c>
-      <c r="E52" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="F52" s="18" t="s">
-        <v>65</v>
+      <c r="E52" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="G52" s="9" t="s">
         <v>9</v>
@@ -5691,30 +5634,30 @@
         <v>2</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K52" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K52" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L52" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B53" s="14" t="s">
+      <c r="A53" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B53" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C53" s="9">
         <v>52</v>
       </c>
-      <c r="E53" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F53" s="18" t="s">
-        <v>163</v>
+      <c r="E53" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>161</v>
       </c>
       <c r="G53" s="9" t="s">
         <v>9</v>
@@ -5723,30 +5666,30 @@
         <v>3</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K53" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K53" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L53" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B54" s="14" t="s">
+      <c r="A54" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B54" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C54" s="9">
         <v>53</v>
       </c>
-      <c r="E54" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F54" s="18" t="s">
-        <v>21</v>
+      <c r="E54" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>19</v>
       </c>
       <c r="G54" s="9" t="s">
         <v>9</v>
@@ -5754,34 +5697,34 @@
       <c r="H54" s="8">
         <v>4</v>
       </c>
-      <c r="I54" s="16" t="s">
-        <v>170</v>
+      <c r="I54" s="12" t="s">
+        <v>168</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K54" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K54" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L54" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B55" s="14" t="s">
+      <c r="A55" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B55" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C55" s="9">
         <v>54</v>
       </c>
-      <c r="E55" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="F55" s="18" t="s">
-        <v>62</v>
+      <c r="E55" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>60</v>
       </c>
       <c r="G55" s="9" t="s">
         <v>9</v>
@@ -5789,34 +5732,34 @@
       <c r="H55" s="8">
         <v>2</v>
       </c>
-      <c r="I55" s="16" t="s">
-        <v>170</v>
+      <c r="I55" s="12" t="s">
+        <v>168</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K55" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K55" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L55" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B56" s="14" t="s">
+      <c r="A56" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B56" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C56" s="9">
         <v>55</v>
       </c>
-      <c r="E56" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="F56" s="18" t="s">
-        <v>142</v>
+      <c r="E56" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>140</v>
       </c>
       <c r="G56" s="9" t="s">
         <v>9</v>
@@ -5824,34 +5767,34 @@
       <c r="H56" s="8">
         <v>1</v>
       </c>
-      <c r="I56" s="16" t="s">
-        <v>165</v>
+      <c r="I56" s="12" t="s">
+        <v>163</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K56" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K56" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L56" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B57" s="14" t="s">
+      <c r="A57" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B57" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C57" s="9">
         <v>56</v>
       </c>
-      <c r="E57" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="F57" s="18" t="s">
-        <v>146</v>
+      <c r="E57" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>144</v>
       </c>
       <c r="G57" s="9" t="s">
         <v>9</v>
@@ -5859,34 +5802,34 @@
       <c r="H57" s="8">
         <v>1</v>
       </c>
-      <c r="I57" s="16" t="s">
-        <v>165</v>
+      <c r="I57" s="12" t="s">
+        <v>163</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K57" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K57" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L57" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B58" s="14" t="s">
+      <c r="A58" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B58" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C58" s="9">
         <v>57</v>
       </c>
-      <c r="E58" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="F58" s="18" t="s">
-        <v>149</v>
+      <c r="E58" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>147</v>
       </c>
       <c r="G58" s="9" t="s">
         <v>9</v>
@@ -5894,34 +5837,34 @@
       <c r="H58" s="8">
         <v>1</v>
       </c>
-      <c r="I58" s="16" t="s">
-        <v>165</v>
+      <c r="I58" s="12" t="s">
+        <v>163</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K58" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K58" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L58" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B59" s="14" t="s">
+      <c r="A59" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B59" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C59" s="9">
         <v>58</v>
       </c>
-      <c r="E59" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="F59" s="18" t="s">
-        <v>118</v>
+      <c r="E59" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="F59" s="13" t="s">
+        <v>116</v>
       </c>
       <c r="G59" s="9" t="s">
         <v>9</v>
@@ -5929,34 +5872,34 @@
       <c r="H59" s="8">
         <v>1</v>
       </c>
-      <c r="I59" s="16" t="s">
-        <v>166</v>
+      <c r="I59" s="12" t="s">
+        <v>164</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K59" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K59" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L59" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B60" s="14" t="s">
+      <c r="A60" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B60" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C60" s="9">
         <v>59</v>
       </c>
-      <c r="E60" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="F60" s="18" t="s">
-        <v>101</v>
+      <c r="E60" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="G60" s="9" t="s">
         <v>9</v>
@@ -5965,30 +5908,30 @@
         <v>1</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K60" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K60" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L60" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B61" s="14" t="s">
+      <c r="A61" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B61" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C61" s="9">
         <v>60</v>
       </c>
-      <c r="E61" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="F61" s="18" t="s">
-        <v>158</v>
+      <c r="E61" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>156</v>
       </c>
       <c r="G61" s="9" t="s">
         <v>9</v>
@@ -5997,27 +5940,27 @@
         <v>1</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K61" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K61" s="14" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B62" s="14" t="s">
+      <c r="A62" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B62" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C62" s="9">
         <v>61</v>
       </c>
-      <c r="E62" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F62" s="18" t="s">
-        <v>90</v>
+      <c r="E62" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="F62" s="13" t="s">
+        <v>88</v>
       </c>
       <c r="G62" s="9" t="s">
         <v>9</v>
@@ -6025,34 +5968,34 @@
       <c r="H62" s="8">
         <v>1</v>
       </c>
-      <c r="I62" s="16" t="s">
-        <v>166</v>
+      <c r="I62" s="12" t="s">
+        <v>164</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K62" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K62" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L62" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B63" s="14" t="s">
+      <c r="A63" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B63" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C63" s="9">
         <v>62</v>
       </c>
-      <c r="E63" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="F63" s="18" t="s">
-        <v>123</v>
+      <c r="E63" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F63" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="G63" s="9" t="s">
         <v>9</v>
@@ -6061,13 +6004,13 @@
         <v>1</v>
       </c>
       <c r="J63" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="K63" s="21" t="s">
-        <v>192</v>
+        <v>162</v>
+      </c>
+      <c r="K63" s="14" t="s">
+        <v>190</v>
       </c>
       <c r="L63" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -6087,7 +6030,7 @@
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId10"/>
   <drawing r:id="rId11"/>
   <webPublishItems count="1">
-    <webPublishItem id="6083" divId="BOM_ZR_V2_6083" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_ZR_V2.5.htm" autoRepublish="1"/>
+    <webPublishItem id="6083" divId="BOM_ZR_V2_6083" sourceType="sheet" destinationFile="C:\Users\olivi\HevORT\bom\BOM_ZR_V2.5.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
     <tablePart r:id="rId12"/>

</xml_diff>